<commit_message>
Text alignment updated, pages modified (Contact, Profile, Add Blog), fields added/changed, data fetched & displayed, button actions updated, and file naming set from user input.
</commit_message>
<xml_diff>
--- a/Daliy report for intership.xlsx
+++ b/Daliy report for intership.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\intership\task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3EDE9E-DE8D-423C-AAC7-27C253071FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD0766A-CB22-458E-945B-11C95437D3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3B151EBB-8F28-4EA9-9DF6-8FD080780458}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Blog app create popup and animation and submit button animation</t>
   </si>
   <si>
-    <t>Learing Skillset</t>
-  </si>
-  <si>
     <t>Html and Bootstrap</t>
   </si>
   <si>
@@ -127,13 +124,72 @@
   </si>
   <si>
     <t>Task Location</t>
+  </si>
+  <si>
+    <t>https://github.com/AakashChidambaranathan/Intership_task/tree/090c27cc40fb24267ff90c66f4345e102283eff9</t>
+  </si>
+  <si>
+    <t>WEEK 1</t>
+  </si>
+  <si>
+    <t>WEEK 2</t>
+  </si>
+  <si>
+    <t>WEEK 3</t>
+  </si>
+  <si>
+    <t>D:\intership\task\first_week\task 1 -change_size_of _text</t>
+  </si>
+  <si>
+    <t>D:\intership\task\first_week\task 2-simple_web_page</t>
+  </si>
+  <si>
+    <t>D:\intership\task\first_week\task_3_Blog_on_react\blog-app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEAVE </t>
+  </si>
+  <si>
+    <t>reasons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date </t>
+  </si>
+  <si>
+    <t>internal exam</t>
+  </si>
+  <si>
+    <t>Learning Skillset</t>
+  </si>
+  <si>
+    <t>Weekly Report</t>
+  </si>
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>This week focused on learning HTML, CSS, JavaScript, Bootstrap, and React, starting from basic Bootstrap concepts to building responsive and interactive blog pages.
+By the end of the week, a blog page was successfully developed using React and Bootstrap, improving skills in UI design and responsiveness.</t>
+  </si>
+  <si>
+    <t>week 2</t>
+  </si>
+  <si>
+    <t>This week focused on enhancing the React blog app by adding popups, animations, UI improvements, and displaying data dynamically from the add blog page.
+One day was taken as leave for CAT exam, while continuous progress was made on React and Bootstrap integration.</t>
+  </si>
+  <si>
+    <t>Holiday</t>
+  </si>
+  <si>
+    <t>Reasons</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +214,21 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -190,7 +261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -206,6 +277,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -522,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D999300A-A676-4830-BF8B-3ED0F14791B7}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="147" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,9 +625,12 @@
     <col min="4" max="4" width="47" customWidth="1"/>
     <col min="5" max="5" width="77.88671875" customWidth="1"/>
     <col min="6" max="6" width="50.5546875" customWidth="1"/>
+    <col min="7" max="7" width="27.77734375" customWidth="1"/>
+    <col min="8" max="8" width="26.77734375" customWidth="1"/>
+    <col min="20" max="20" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -549,124 +641,175 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="10"/>
+      <c r="T1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" s="10"/>
+      <c r="V1" s="6"/>
+      <c r="X1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y1" s="10"/>
+    </row>
+    <row r="2" spans="1:25" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B2" s="8"/>
+      <c r="C2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" s="6"/>
+      <c r="X2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>45992</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="6"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>45992</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="3">
+        <v>46001</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+    </row>
+    <row r="4" spans="1:25" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>45993</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="E4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="12"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+    </row>
+    <row r="5" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>45994</v>
+      </c>
+      <c r="B5" s="9">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>45993</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>45995</v>
+      </c>
+      <c r="B6" s="9">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>45994</v>
-      </c>
-      <c r="B4" s="2">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>45995</v>
-      </c>
-      <c r="B5" s="2">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="12"/>
+    </row>
+    <row r="7" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>45996</v>
+      </c>
+      <c r="B7" s="9">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>45996</v>
-      </c>
-      <c r="B6" s="2">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>45997</v>
       </c>
-      <c r="B7" s="2">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>45998</v>
-      </c>
-      <c r="B8" s="2">
-        <v>7</v>
+      <c r="B8" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
@@ -674,193 +817,222 @@
       <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E8" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
+        <v>45998</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B10" s="8"/>
+      <c r="C10" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>45999</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B11" s="9">
+        <v>6</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>46000</v>
+      </c>
+      <c r="B12" s="9">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>46001</v>
+      </c>
+      <c r="B13" s="9">
         <v>8</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="7" t="s">
+      <c r="C13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>46002</v>
+      </c>
+      <c r="B14" s="9">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>46000</v>
-      </c>
-      <c r="B10" s="2">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>46001</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>46003</v>
+      </c>
+      <c r="B15" s="9">
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>46004</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>46002</v>
-      </c>
-      <c r="B12" s="2">
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>46005</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B18" s="8"/>
+      <c r="C18" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>46006</v>
+      </c>
+      <c r="B19" s="9">
         <v>11</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>46003</v>
-      </c>
-      <c r="B13" s="2">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>46004</v>
-      </c>
-      <c r="B14" s="2">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
-        <v>46005</v>
-      </c>
-      <c r="B15" s="2">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>46006</v>
-      </c>
-      <c r="B16" s="2">
-        <v>15</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
-        <v>46007</v>
-      </c>
-      <c r="B17" s="2">
-        <v>16</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -868,18 +1040,25 @@
       <c r="E23" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="H11:H15"/>
+    <mergeCell ref="X1:Y1"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C9" r:id="rId1" tooltip="Day -7 Blog app create popup and animation" display="https://github.com/AakashChidambaranathan/Intership_task/commit/47e9946674f87f428e5d2cff5875e3cca658dd67" xr:uid="{2740968A-86F6-4ABB-8E7C-25250927D97F}"/>
-    <hyperlink ref="E2" r:id="rId2" display="https://github.com/AakashChidambaranathan/Intership_task/tree/b173e2d43ecb1fd92e9d3f8ea145f4a80c1ea62c" xr:uid="{BF70E11B-AFAF-45B3-AA62-D198D53E94AC}"/>
-    <hyperlink ref="E3" r:id="rId3" display="https://github.com/AakashChidambaranathan/Intership_task/tree/b173e2d43ecb1fd92e9d3f8ea145f4a80c1ea62c" xr:uid="{112BC480-767B-4896-84B0-1E49BB3C0F10}"/>
-    <hyperlink ref="E4" r:id="rId4" display="https://github.com/AakashChidambaranathan/Intership_task/tree/492c28a482b2757a441e3dbc986bf024969d1e78" xr:uid="{97DD4FE9-8689-492F-9396-D336CB3CC87C}"/>
-    <hyperlink ref="E5" r:id="rId5" display="https://github.com/AakashChidambaranathan/Intership_task/tree/4d8e8c4efe1c4d6c2951e9567b5a30fd9753930f" xr:uid="{59F50829-1528-4798-B383-ECBE692F3DFB}"/>
-    <hyperlink ref="E6" r:id="rId6" display="https://github.com/AakashChidambaranathan/Intership_task/tree/0219356c732cd4e6a9f90160fbb3aa0095e6ad70" xr:uid="{BE17C8CD-A0E4-40B5-810D-2AABF44AA421}"/>
-    <hyperlink ref="E9" r:id="rId7" display="https://github.com/AakashChidambaranathan/Intership_task/tree/fabb22e71f0786d4df5ddba16ff5e56255455d94" xr:uid="{16D6FD75-ABAF-4F19-8D25-CFED163DEB53}"/>
-    <hyperlink ref="E10" r:id="rId8" display="https://github.com/AakashChidambaranathan/Intership_task/tree/fabb22e71f0786d4df5ddba16ff5e56255455d94" xr:uid="{B68916E8-A3E3-4B91-B9CC-D62094D9470B}"/>
-    <hyperlink ref="E12" r:id="rId9" display="https://github.com/AakashChidambaranathan/Intership_task/tree/f8d6a572c3bd2738f9f29acd251ec176e69bb852" xr:uid="{07CDCB6E-5262-4EED-A54B-AE7617BE6248}"/>
-    <hyperlink ref="E13" r:id="rId10" display="https://github.com/AakashChidambaranathan/Intership_task/tree/99b5f9cb065f0c3226b532596a7ec487a3f9dbcf" xr:uid="{463AFCAE-8D2D-417D-A565-BBA915E923A6}"/>
-    <hyperlink ref="E16" r:id="rId11" display="https://github.com/AakashChidambaranathan/Intership_task/tree/99b5f9cb065f0c3226b532596a7ec487a3f9dbcf" xr:uid="{2609AE2F-9ED4-457D-90C5-69E3CB1E14D6}"/>
+    <hyperlink ref="C11" r:id="rId1" tooltip="Day -7 Blog app create popup and animation" display="https://github.com/AakashChidambaranathan/Intership_task/commit/47e9946674f87f428e5d2cff5875e3cca658dd67" xr:uid="{2740968A-86F6-4ABB-8E7C-25250927D97F}"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://github.com/AakashChidambaranathan/Intership_task/tree/b173e2d43ecb1fd92e9d3f8ea145f4a80c1ea62c" xr:uid="{BF70E11B-AFAF-45B3-AA62-D198D53E94AC}"/>
+    <hyperlink ref="E4" r:id="rId3" display="https://github.com/AakashChidambaranathan/Intership_task/tree/b173e2d43ecb1fd92e9d3f8ea145f4a80c1ea62c" xr:uid="{112BC480-767B-4896-84B0-1E49BB3C0F10}"/>
+    <hyperlink ref="E5" r:id="rId4" display="https://github.com/AakashChidambaranathan/Intership_task/tree/492c28a482b2757a441e3dbc986bf024969d1e78" xr:uid="{97DD4FE9-8689-492F-9396-D336CB3CC87C}"/>
+    <hyperlink ref="E6" r:id="rId5" display="https://github.com/AakashChidambaranathan/Intership_task/tree/4d8e8c4efe1c4d6c2951e9567b5a30fd9753930f" xr:uid="{59F50829-1528-4798-B383-ECBE692F3DFB}"/>
+    <hyperlink ref="E7" r:id="rId6" display="https://github.com/AakashChidambaranathan/Intership_task/tree/0219356c732cd4e6a9f90160fbb3aa0095e6ad70" xr:uid="{BE17C8CD-A0E4-40B5-810D-2AABF44AA421}"/>
+    <hyperlink ref="E11" r:id="rId7" display="https://github.com/AakashChidambaranathan/Intership_task/tree/fabb22e71f0786d4df5ddba16ff5e56255455d94" xr:uid="{16D6FD75-ABAF-4F19-8D25-CFED163DEB53}"/>
+    <hyperlink ref="E12" r:id="rId8" display="https://github.com/AakashChidambaranathan/Intership_task/tree/fabb22e71f0786d4df5ddba16ff5e56255455d94" xr:uid="{B68916E8-A3E3-4B91-B9CC-D62094D9470B}"/>
+    <hyperlink ref="E14" r:id="rId9" display="https://github.com/AakashChidambaranathan/Intership_task/tree/f8d6a572c3bd2738f9f29acd251ec176e69bb852" xr:uid="{07CDCB6E-5262-4EED-A54B-AE7617BE6248}"/>
+    <hyperlink ref="E15" r:id="rId10" display="https://github.com/AakashChidambaranathan/Intership_task/tree/99b5f9cb065f0c3226b532596a7ec487a3f9dbcf" xr:uid="{463AFCAE-8D2D-417D-A565-BBA915E923A6}"/>
+    <hyperlink ref="E19" r:id="rId11" xr:uid="{2609AE2F-9ED4-457D-90C5-69E3CB1E14D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Express and JSON we need to store a data on json file on public folder
</commit_message>
<xml_diff>
--- a/Daliy report for intership.xlsx
+++ b/Daliy report for intership.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\intership\task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1357741-EB21-4E76-B74C-456D5329323D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4488E6BD-2108-43D1-B2D9-BBAEFA3EC838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3B151EBB-8F28-4EA9-9DF6-8FD080780458}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
   <si>
     <t>Date</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Start learning react and complect one page on blog</t>
   </si>
   <si>
-    <t>I completed one page using React and Bootstrap, and I’m also learning Bootstrap as part of the process.</t>
-  </si>
-  <si>
     <t>holiday</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>Blog app Change ui for add blog page</t>
   </si>
   <si>
-    <t>create page display data from add blog page</t>
-  </si>
-  <si>
     <t>Blog app create popup and animation and submit button animation</t>
   </si>
   <si>
@@ -123,21 +117,9 @@
     <t>-</t>
   </si>
   <si>
-    <t>Task Location</t>
-  </si>
-  <si>
     <t>https://github.com/AakashChidambaranathan/Intership_task/tree/090c27cc40fb24267ff90c66f4345e102283eff9</t>
   </si>
   <si>
-    <t>WEEK 1</t>
-  </si>
-  <si>
-    <t>WEEK 2</t>
-  </si>
-  <si>
-    <t>WEEK 3</t>
-  </si>
-  <si>
     <t>D:\intership\task\first_week\task 1 -change_size_of _text</t>
   </si>
   <si>
@@ -154,9 +136,6 @@
   </si>
   <si>
     <t xml:space="preserve">Date </t>
-  </si>
-  <si>
-    <t>internal exam</t>
   </si>
   <si>
     <t>Learning Skillset</t>
@@ -198,13 +177,124 @@
   </si>
   <si>
     <t>Week 3</t>
+  </si>
+  <si>
+    <t>learn express and middleware</t>
+  </si>
+  <si>
+    <t>React and node.js</t>
+  </si>
+  <si>
+    <t>AakashChidambaranathan/Intership_task at 2dd6098d3b32e05b05fd6d455f18f7de6abae75d</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WEEK 2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(REACT AND BOOTSTRAP)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WEEK 1  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(HTML,CSS AND JS)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WEEK 3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(REACT AND NODE.JS)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>WORKING DAYS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t>Attend</t>
+  </si>
+  <si>
+    <t>Internal exam</t>
+  </si>
+  <si>
+    <t>Express and json</t>
+  </si>
+  <si>
+    <t>Express and JSON (we need to store a data on json file on public folderder) --- (work form home)</t>
+  </si>
+  <si>
+    <t>create page display data from add blog page-- (work from home)</t>
+  </si>
+  <si>
+    <t>I completed one page using React and Bootstrap, and I’m also learning Bootstrap as part of the process.--(work from home)</t>
+  </si>
+  <si>
+    <t>Weekly skills learning</t>
+  </si>
+  <si>
+    <t>Week No</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Learning</t>
+  </si>
+  <si>
+    <t>week 1</t>
+  </si>
+  <si>
+    <t>week 3</t>
+  </si>
+  <si>
+    <t>react nad Bootstrap</t>
+  </si>
+  <si>
+    <t>react and node.js</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Task System Location</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +338,18 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -276,7 +378,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -302,6 +404,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -311,7 +426,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -627,15 +741,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D999300A-A676-4830-BF8B-3ED0F14791B7}">
-  <dimension ref="A1:Y24"/>
+  <dimension ref="A1:AC24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="116" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="78" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="95.33203125" customWidth="1"/>
     <col min="4" max="4" width="47" customWidth="1"/>
@@ -643,62 +757,97 @@
     <col min="6" max="6" width="50.5546875" customWidth="1"/>
     <col min="7" max="7" width="27.77734375" customWidth="1"/>
     <col min="8" max="8" width="26.77734375" customWidth="1"/>
-    <col min="20" max="20" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" customWidth="1"/>
+    <col min="19" max="19" width="7.88671875" customWidth="1"/>
+    <col min="20" max="20" width="12.77734375" customWidth="1"/>
+    <col min="21" max="21" width="12.88671875" customWidth="1"/>
+    <col min="22" max="22" width="15.21875" customWidth="1"/>
+    <col min="24" max="24" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.21875" customWidth="1"/>
+    <col min="27" max="27" width="7.6640625" customWidth="1"/>
+    <col min="28" max="28" width="11" customWidth="1"/>
+    <col min="29" max="29" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="M1" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="16"/>
+      <c r="S1" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="6"/>
+      <c r="X1" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y1" s="16"/>
+      <c r="AB1" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC1" s="17"/>
+    </row>
+    <row r="2" spans="1:29" ht="18" x14ac:dyDescent="0.35">
+      <c r="B2" s="8"/>
+      <c r="C2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="V2" s="6"/>
+      <c r="X2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="12"/>
-      <c r="T1" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="U1" s="12"/>
-      <c r="V1" s="6"/>
-      <c r="X1" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y1" s="12"/>
-    </row>
-    <row r="2" spans="1:25" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B2" s="8"/>
-      <c r="C2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="V2" s="6"/>
-      <c r="X2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="AB2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>45992</v>
       </c>
@@ -706,30 +855,51 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="N3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="T3" s="3">
+      <c r="O3" s="2"/>
+      <c r="S3" s="9">
+        <v>1</v>
+      </c>
+      <c r="T3" s="14">
         <v>46001</v>
       </c>
-      <c r="U3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-    </row>
-    <row r="4" spans="1:25" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="U3" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="X3" s="14">
+        <v>45997</v>
+      </c>
+      <c r="Y3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB3" s="9">
+        <v>15</v>
+      </c>
+      <c r="AC3" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>45993</v>
       </c>
@@ -739,22 +909,37 @@
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
+      <c r="D4" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="14"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-    </row>
-    <row r="5" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="19"/>
+      <c r="M4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="X4" s="14">
+        <v>45998</v>
+      </c>
+      <c r="Y4" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+    </row>
+    <row r="5" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>45994</v>
       </c>
@@ -764,21 +949,36 @@
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
+      <c r="D5" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="14"/>
-    </row>
-    <row r="6" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="M5" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="X5" s="14">
+        <v>46004</v>
+      </c>
+      <c r="Y5" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>45995</v>
       </c>
@@ -788,18 +988,30 @@
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>15</v>
+      <c r="D6" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="14"/>
-    </row>
-    <row r="7" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="19"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="2"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="X6" s="14">
+        <v>46005</v>
+      </c>
+      <c r="Y6" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>45996</v>
       </c>
@@ -807,60 +1019,79 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>63</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="14"/>
-    </row>
-    <row r="8" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="19"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+    </row>
+    <row r="8" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>45997</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+    </row>
+    <row r="9" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>45998</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="18" x14ac:dyDescent="0.35">
       <c r="B10" s="8"/>
-      <c r="C10" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C10" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="V10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>45999</v>
       </c>
@@ -868,22 +1099,23 @@
         <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>46000</v>
       </c>
@@ -891,20 +1123,21 @@
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="15"/>
-    </row>
-    <row r="13" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="G12" s="17"/>
+      <c r="H12" s="20"/>
+    </row>
+    <row r="13" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>46001</v>
       </c>
@@ -912,20 +1145,20 @@
         <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="G13" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="15"/>
-    </row>
-    <row r="14" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="H13" s="20"/>
+    </row>
+    <row r="14" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>46002</v>
       </c>
@@ -933,20 +1166,21 @@
         <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="G14" s="17"/>
+      <c r="H14" s="20"/>
+    </row>
+    <row r="15" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>46003</v>
       </c>
@@ -954,60 +1188,68 @@
         <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>17</v>
+        <v>62</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="15"/>
-    </row>
-    <row r="16" spans="1:25" ht="15.6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="20"/>
+    </row>
+    <row r="16" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>46004</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>46005</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B18" s="8"/>
-      <c r="C18" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C18" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>46006</v>
       </c>
@@ -1015,19 +1257,21 @@
         <v>11</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" t="s">
         <v>30</v>
       </c>
-      <c r="F19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>46007</v>
       </c>
@@ -1037,67 +1281,99 @@
       <c r="C20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>17</v>
+      <c r="D20" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>46008</v>
       </c>
       <c r="B21" s="9">
         <v>13</v>
       </c>
-      <c r="C21" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>17</v>
+      <c r="C21" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="H21" s="17"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>46009</v>
       </c>
       <c r="B22" s="9">
         <v>14</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" s="17"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>46010</v>
       </c>
       <c r="B23" s="9">
         <v>15</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B24" s="8"/>
+      <c r="D24" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="T1:U1"/>
+  <mergeCells count="14">
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="H19:H23"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="S1:U1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="H3:H7"/>
     <mergeCell ref="H11:H15"/>
@@ -1118,6 +1394,7 @@
     <hyperlink ref="E20" r:id="rId12" display="https://github.com/AakashChidambaranathan/Intership_task/tree/f2e646fc76a8ead55f6b5c582100ae58d402bfa0" xr:uid="{BB4C039B-EF43-477E-B5F1-C5365A6E7603}"/>
     <hyperlink ref="C21" r:id="rId13" tooltip="dynamic change text" display="https://github.com/AakashChidambaranathan/Intership_task/commit/b1ca1109002a654f7551b2c3c0e56c48460bf95e" xr:uid="{83C49FAA-695C-44FD-9C0C-3B478D02274C}"/>
     <hyperlink ref="E21" r:id="rId14" xr:uid="{F14A6C10-B97A-47DA-80B2-72AD31150AF1}"/>
+    <hyperlink ref="E22" r:id="rId15" display="https://github.com/AakashChidambaranathan/Intership_task/tree/2dd6098d3b32e05b05fd6d455f18f7de6abae75d" xr:uid="{64C600C4-AF47-4FB7-954C-5BC7AEBEF4BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
22-dec Store data in json file
</commit_message>
<xml_diff>
--- a/Daliy report for intership.xlsx
+++ b/Daliy report for intership.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\intership\task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4488E6BD-2108-43D1-B2D9-BBAEFA3EC838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211962CC-0CB9-458E-9952-C6A67E656972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3B151EBB-8F28-4EA9-9DF6-8FD080780458}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -288,6 +288,12 @@
   </si>
   <si>
     <t>Task System Location</t>
+  </si>
+  <si>
+    <t>AakashChidambaranathan/Intership_task at 8702c10b09067fcb834f14066909a04ddc83680e</t>
+  </si>
+  <si>
+    <t>During this week, I developed and enhanced a blog application using React and Bootstrap by adding popups, animations, responsive design, interactive features, and dynamic text updates. I also learned and worked with Node.js and Express, including middleware concepts and storing application data in JSON files, with hands-on practice and work-from-home tasks.</t>
   </si>
 </sst>
 </file>
@@ -743,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D999300A-A676-4830-BF8B-3ED0F14791B7}">
   <dimension ref="A1:AC24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="78" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="F2" zoomScale="110" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1034,8 +1040,12 @@
       <c r="H7" s="19"/>
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
+      <c r="X7" s="14">
+        <v>46011</v>
+      </c>
+      <c r="Y7" s="9" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
@@ -1058,8 +1068,12 @@
       </c>
       <c r="M8" s="12"/>
       <c r="N8" s="12"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
+      <c r="X8" s="14">
+        <v>46012</v>
+      </c>
+      <c r="Y8" s="9" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
@@ -1269,7 +1283,9 @@
         <v>30</v>
       </c>
       <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="H19" s="18" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
@@ -1291,7 +1307,7 @@
         <v>30</v>
       </c>
       <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="21" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
@@ -1315,7 +1331,7 @@
       <c r="G21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="17"/>
+      <c r="H21" s="20"/>
     </row>
     <row r="22" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
@@ -1339,7 +1355,7 @@
       <c r="G22" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="17"/>
+      <c r="H22" s="20"/>
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
@@ -1354,9 +1370,14 @@
       <c r="D23" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" t="s">
+        <v>45</v>
+      </c>
       <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
+      <c r="H23" s="20"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B24" s="8"/>
@@ -1395,6 +1416,7 @@
     <hyperlink ref="C21" r:id="rId13" tooltip="dynamic change text" display="https://github.com/AakashChidambaranathan/Intership_task/commit/b1ca1109002a654f7551b2c3c0e56c48460bf95e" xr:uid="{83C49FAA-695C-44FD-9C0C-3B478D02274C}"/>
     <hyperlink ref="E21" r:id="rId14" xr:uid="{F14A6C10-B97A-47DA-80B2-72AD31150AF1}"/>
     <hyperlink ref="E22" r:id="rId15" display="https://github.com/AakashChidambaranathan/Intership_task/tree/2dd6098d3b32e05b05fd6d455f18f7de6abae75d" xr:uid="{64C600C4-AF47-4FB7-954C-5BC7AEBEF4BF}"/>
+    <hyperlink ref="E23" r:id="rId16" display="https://github.com/AakashChidambaranathan/Intership_task/tree/8702c10b09067fcb834f14066909a04ddc83680e" xr:uid="{14736496-F2DA-481F-9D9D-5AB3AE7C15C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
json store a data from form
</commit_message>
<xml_diff>
--- a/Daliy report for intership.xlsx
+++ b/Daliy report for intership.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\intership\task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211962CC-0CB9-458E-9952-C6A67E656972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2207B91E-F5E1-4F18-BFFD-92CA4073B62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3B151EBB-8F28-4EA9-9DF6-8FD080780458}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="77">
   <si>
     <t>Date</t>
   </si>
@@ -294,6 +294,12 @@
   </si>
   <si>
     <t>During this week, I developed and enhanced a blog application using React and Bootstrap by adding popups, animations, responsive design, interactive features, and dynamic text updates. I also learned and worked with Node.js and Express, including middleware concepts and storing application data in JSON files, with hands-on practice and work-from-home tasks.</t>
+  </si>
+  <si>
+    <t>Express and JSON (we need to store a data on json file on public folderder)</t>
+  </si>
+  <si>
+    <t>AakashChidambaranathan/Intership_task at 2385d676f720ebd8a58de01590373056baf3a957</t>
   </si>
 </sst>
 </file>
@@ -426,10 +432,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -747,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D999300A-A676-4830-BF8B-3ED0F14791B7}">
-  <dimension ref="A1:AC24"/>
+  <dimension ref="A1:AC30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" zoomScale="110" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="93" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -925,7 +931,7 @@
         <v>28</v>
       </c>
       <c r="G4" s="17"/>
-      <c r="H4" s="19"/>
+      <c r="H4" s="20"/>
       <c r="M4" s="9" t="s">
         <v>38</v>
       </c>
@@ -967,7 +973,7 @@
       <c r="G5" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="19"/>
+      <c r="H5" s="20"/>
       <c r="M5" s="9" t="s">
         <v>68</v>
       </c>
@@ -1004,7 +1010,7 @@
         <v>30</v>
       </c>
       <c r="G6" s="17"/>
-      <c r="H6" s="19"/>
+      <c r="H6" s="20"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
       <c r="O6" s="2"/>
@@ -1037,7 +1043,7 @@
         <v>30</v>
       </c>
       <c r="G7" s="17"/>
-      <c r="H7" s="19"/>
+      <c r="H7" s="20"/>
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
       <c r="X7" s="14">
@@ -1149,7 +1155,7 @@
         <v>30</v>
       </c>
       <c r="G12" s="17"/>
-      <c r="H12" s="20"/>
+      <c r="H12" s="19"/>
     </row>
     <row r="13" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
@@ -1170,7 +1176,7 @@
       <c r="G13" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="20"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
@@ -1192,7 +1198,7 @@
         <v>30</v>
       </c>
       <c r="G14" s="17"/>
-      <c r="H14" s="20"/>
+      <c r="H14" s="19"/>
     </row>
     <row r="15" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
@@ -1214,7 +1220,7 @@
         <v>30</v>
       </c>
       <c r="G15" s="17"/>
-      <c r="H15" s="20"/>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
@@ -1307,7 +1313,7 @@
         <v>30</v>
       </c>
       <c r="G20" s="17"/>
-      <c r="H20" s="20"/>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
@@ -1331,7 +1337,7 @@
       <c r="G21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="20"/>
+      <c r="H21" s="19"/>
     </row>
     <row r="22" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
@@ -1355,7 +1361,7 @@
       <c r="G22" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="20"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
@@ -1377,11 +1383,99 @@
         <v>45</v>
       </c>
       <c r="G23" s="17"/>
-      <c r="H23" s="20"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="8"/>
-      <c r="D24" s="8"/>
+      <c r="H23" s="19"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>46011</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>46012</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>46013</v>
+      </c>
+      <c r="B26" s="9">
+        <v>16</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>46014</v>
+      </c>
+      <c r="B27" s="9">
+        <v>17</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>46015</v>
+      </c>
+      <c r="B28" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>46016</v>
+      </c>
+      <c r="B29" s="9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>46017</v>
+      </c>
+      <c r="B30" s="9">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -1417,6 +1511,7 @@
     <hyperlink ref="E21" r:id="rId14" xr:uid="{F14A6C10-B97A-47DA-80B2-72AD31150AF1}"/>
     <hyperlink ref="E22" r:id="rId15" display="https://github.com/AakashChidambaranathan/Intership_task/tree/2dd6098d3b32e05b05fd6d455f18f7de6abae75d" xr:uid="{64C600C4-AF47-4FB7-954C-5BC7AEBEF4BF}"/>
     <hyperlink ref="E23" r:id="rId16" display="https://github.com/AakashChidambaranathan/Intership_task/tree/8702c10b09067fcb834f14066909a04ddc83680e" xr:uid="{14736496-F2DA-481F-9D9D-5AB3AE7C15C3}"/>
+    <hyperlink ref="E26" r:id="rId17" display="https://github.com/AakashChidambaranathan/Intership_task/tree/2385d676f720ebd8a58de01590373056baf3a957" xr:uid="{F0BDF0C3-BC66-4764-9A83-13AAB2D059C6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
try_crud_opertion on node js
</commit_message>
<xml_diff>
--- a/Daliy report for intership.xlsx
+++ b/Daliy report for intership.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\intership\task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2207B91E-F5E1-4F18-BFFD-92CA4073B62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BFADAB-567B-4385-B816-B5BD3A183ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3B151EBB-8F28-4EA9-9DF6-8FD080780458}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="78">
   <si>
     <t>Date</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t>AakashChidambaranathan/Intership_task at 2385d676f720ebd8a58de01590373056baf3a957</t>
+  </si>
+  <si>
+    <t>AakashChidambaranathan/Intership_task at 0470b045f604410b0cb1eeecd44a8d810df89475</t>
   </si>
 </sst>
 </file>
@@ -755,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D999300A-A676-4830-BF8B-3ED0F14791B7}">
   <dimension ref="A1:AC30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="93" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="93" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="D28" activeCellId="1" sqref="E27 D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1451,6 +1454,9 @@
       </c>
       <c r="D27" s="9" t="s">
         <v>60</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -1512,6 +1518,7 @@
     <hyperlink ref="E22" r:id="rId15" display="https://github.com/AakashChidambaranathan/Intership_task/tree/2dd6098d3b32e05b05fd6d455f18f7de6abae75d" xr:uid="{64C600C4-AF47-4FB7-954C-5BC7AEBEF4BF}"/>
     <hyperlink ref="E23" r:id="rId16" display="https://github.com/AakashChidambaranathan/Intership_task/tree/8702c10b09067fcb834f14066909a04ddc83680e" xr:uid="{14736496-F2DA-481F-9D9D-5AB3AE7C15C3}"/>
     <hyperlink ref="E26" r:id="rId17" display="https://github.com/AakashChidambaranathan/Intership_task/tree/2385d676f720ebd8a58de01590373056baf3a957" xr:uid="{F0BDF0C3-BC66-4764-9A83-13AAB2D059C6}"/>
+    <hyperlink ref="E27" r:id="rId18" display="https://github.com/AakashChidambaranathan/Intership_task/tree/0470b045f604410b0cb1eeecd44a8d810df89475" xr:uid="{53DA9962-094B-4F7E-B20F-CD07E8D4391B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Profile page updation and store a data on both json and txt
</commit_message>
<xml_diff>
--- a/Daliy report for intership.xlsx
+++ b/Daliy report for intership.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\intership\task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79237247-DEA0-496F-B9B2-657B53ED2DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9021F2B6-4AB4-495D-AC56-CECCF7A3854B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3B151EBB-8F28-4EA9-9DF6-8FD080780458}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Full report" sheetId="1" r:id="rId1"/>
+    <sheet name="December " sheetId="2" r:id="rId2"/>
+    <sheet name="Weekly Learning" sheetId="4" r:id="rId3"/>
+    <sheet name="Attentancs" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="108">
   <si>
     <t>Date</t>
   </si>
@@ -338,12 +341,104 @@
   <si>
     <t>christmas holiday</t>
   </si>
+  <si>
+    <t>AakashChidambaranathan/Intership_task at 5e82dcb38869f9dae5bf244ad47810f0bde98f7d</t>
+  </si>
+  <si>
+    <t>Express and JSON (File operation)</t>
+  </si>
+  <si>
+    <t>AakashChidambaranathan/Intership_task at 9135683980ad23825bb62e52e371e0f6e3c013c4</t>
+  </si>
+  <si>
+    <t>Express and JSON (File opreation) --- (work form home)</t>
+  </si>
+  <si>
+    <t>Node.js</t>
+  </si>
+  <si>
+    <t>Try CRUD Opertion on node js</t>
+  </si>
+  <si>
+    <t>AakashChidambaranathan/Intership_task at c0f18dc48dfe3188a657f8099cc04fcddf58a7e0</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WEEK 6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(REACT AND NODE.JS)</t>
+    </r>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Server Updatation </t>
+  </si>
+  <si>
+    <t>Express and JSON (updata profile page and data store both text file and json file)</t>
+  </si>
+  <si>
+    <t>During this week, I worked with Express.js and JSON to store and manage data in a public folder.I also practiced CRUD operations using Node.js to create, read, update, and delete data.
+This work helped me understand backend development and server-side data handling.</t>
+  </si>
+  <si>
+    <t>During this period, I worked on server updates using Node.js to improve backend functionality.
+I also performed file operations using Express.js and JSON while working from home.
+These tasks helped me understand server maintenance and data handling in backend development.</t>
+  </si>
+  <si>
+    <t>week 4</t>
+  </si>
+  <si>
+    <t>week 5</t>
+  </si>
+  <si>
+    <t>Node.js ,express js,JSON,CRUD Opretion</t>
+  </si>
+  <si>
+    <t>Node.js,Express.js,JSON File,Operations,Server Update &amp; Maintenance</t>
+  </si>
+  <si>
+    <t>Try CRUD Opertion on node js --- (work form home)</t>
+  </si>
+  <si>
+    <t>Notes link(Github)</t>
+  </si>
+  <si>
+    <t>Cors: https://github.com/AakashChidambaranathan/Intership_task/blob/main/Notes/NodeJs/cors.txt  file_System(method):https://github.com/AakashChidambaranathan/Intership_task/blob/main/Notes/NodeJs/file_System(method).txt</t>
+  </si>
+  <si>
+    <t>WORKING DAYS (Upto 06-01-2026)</t>
+  </si>
+  <si>
+    <t>Technology Used</t>
+  </si>
+  <si>
+    <t>Task Description</t>
+  </si>
+  <si>
+    <t>Reference  (GitHub Commit)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,14 +469,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -398,6 +485,25 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman\"/>
     </font>
   </fonts>
   <fills count="3">
@@ -427,7 +533,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -435,19 +541,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -457,13 +554,25 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -472,10 +581,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -791,25 +930,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D999300A-A676-4830-BF8B-3ED0F14791B7}">
-  <dimension ref="A1:AC37"/>
+  <dimension ref="A1:AC47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="95.33203125" customWidth="1"/>
     <col min="4" max="4" width="47" customWidth="1"/>
     <col min="5" max="5" width="77.88671875" customWidth="1"/>
     <col min="6" max="6" width="50.5546875" customWidth="1"/>
     <col min="7" max="7" width="27.77734375" customWidth="1"/>
-    <col min="8" max="8" width="26.77734375" customWidth="1"/>
+    <col min="8" max="8" width="52.77734375" customWidth="1"/>
     <col min="12" max="12" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" customWidth="1"/>
-    <col min="14" max="14" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="20.109375" customWidth="1"/>
+    <col min="14" max="14" width="53.21875" customWidth="1"/>
     <col min="19" max="19" width="7.88671875" customWidth="1"/>
     <col min="20" max="20" width="12.77734375" customWidth="1"/>
     <col min="21" max="21" width="12.88671875" customWidth="1"/>
@@ -821,806 +960,1121 @@
     <col min="29" max="29" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:29" ht="17.399999999999999">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="12" t="s">
+      <c r="C1" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="M1" s="16" t="s">
+      <c r="H1" s="20"/>
+      <c r="M1" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="16"/>
-      <c r="S1" s="16" t="s">
+      <c r="N1" s="20"/>
+      <c r="S1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
       <c r="V1" s="6"/>
-      <c r="X1" s="16" t="s">
+      <c r="X1" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" s="16"/>
-      <c r="AB1" s="16" t="s">
+      <c r="Y1" s="20"/>
+      <c r="AB1" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="AC1" s="17"/>
-    </row>
-    <row r="2" spans="1:29" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="8"/>
-      <c r="C2" s="12" t="s">
+      <c r="AC1" s="19"/>
+    </row>
+    <row r="2" spans="1:29" ht="18">
+      <c r="A2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="M2" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="S2" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="T2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="U2" s="9" t="s">
         <v>32</v>
       </c>
       <c r="V2" s="6"/>
-      <c r="X2" s="12" t="s">
+      <c r="X2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="Y2" s="12" t="s">
+      <c r="Y2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="9" t="s">
+      <c r="AB2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="AC2" s="9" t="s">
+      <c r="AC2" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="15.6">
       <c r="A3" s="3">
         <v>45992</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="7">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="18" t="s">
+      <c r="G3" s="18"/>
+      <c r="H3" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="O3" s="2"/>
-      <c r="S3" s="9">
+      <c r="S3" s="7">
         <v>1</v>
       </c>
-      <c r="T3" s="14">
+      <c r="T3" s="11">
         <v>46001</v>
       </c>
-      <c r="U3" s="9" t="s">
+      <c r="U3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="X3" s="14">
+      <c r="X3" s="11">
         <v>45997</v>
       </c>
-      <c r="Y3" s="9" t="s">
+      <c r="Y3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="AB3" s="9">
-        <v>15</v>
-      </c>
-      <c r="AC3" s="9">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AB3" s="7">
+        <v>25</v>
+      </c>
+      <c r="AC3" s="7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="15.6">
       <c r="A4" s="3">
         <v>45993</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="7">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="20"/>
-      <c r="M4" s="9" t="s">
+      <c r="G4" s="18"/>
+      <c r="H4" s="23"/>
+      <c r="M4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="N4" s="7" t="s">
         <v>69</v>
       </c>
       <c r="O4" s="2"/>
-      <c r="S4" s="9">
+      <c r="S4" s="7">
         <v>2</v>
       </c>
-      <c r="T4" s="14">
+      <c r="T4" s="11">
         <v>46022</v>
       </c>
-      <c r="U4" s="9" t="s">
+      <c r="U4" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="X4" s="14">
+      <c r="X4" s="11">
         <v>45998</v>
       </c>
-      <c r="Y4" s="9" t="s">
+      <c r="Y4" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-    </row>
-    <row r="5" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="7"/>
+    </row>
+    <row r="5" spans="1:29" ht="15.6">
       <c r="A5" s="3">
         <v>45994</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="7">
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="M5" s="9" t="s">
+      <c r="H5" s="23"/>
+      <c r="M5" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="N5" s="7" t="s">
         <v>70</v>
       </c>
       <c r="O5" s="2"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="X5" s="14">
+      <c r="S5" s="7">
+        <v>3</v>
+      </c>
+      <c r="T5" s="11">
+        <v>46023</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="X5" s="11">
         <v>46004</v>
       </c>
-      <c r="Y5" s="9" t="s">
+      <c r="Y5" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="15.6">
       <c r="A6" s="3">
         <v>45995</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="20"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="23"/>
+      <c r="M6" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>99</v>
+      </c>
       <c r="O6" s="2"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="X6" s="14">
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="X6" s="11">
         <v>46005</v>
       </c>
-      <c r="Y6" s="9" t="s">
+      <c r="Y6" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" ht="18" customHeight="1">
       <c r="A7" s="3">
         <v>45996</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="7">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="20"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="X7" s="14">
+      <c r="G7" s="18"/>
+      <c r="H7" s="23"/>
+      <c r="M7" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="N7" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="X7" s="11">
         <v>46011</v>
       </c>
-      <c r="Y7" s="9" t="s">
+      <c r="Y7" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" ht="17.399999999999999">
       <c r="A8" s="3">
         <v>45997</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="X8" s="14">
+      <c r="B8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="26"/>
+      <c r="X8" s="11">
         <v>46012</v>
       </c>
-      <c r="Y8" s="9" t="s">
+      <c r="Y8" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="15.6">
       <c r="A9" s="3">
         <v>45998</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="X9" s="14">
+      <c r="B9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="N9" s="26"/>
+      <c r="X9" s="11">
         <v>46016</v>
       </c>
-      <c r="Y9" s="9" t="s">
+      <c r="Y9" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="18" x14ac:dyDescent="0.35">
-      <c r="B10" s="8"/>
-      <c r="C10" s="12" t="s">
+    <row r="10" spans="1:29" ht="18">
+      <c r="A10" s="13"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="N10" s="26"/>
       <c r="V10" t="s">
         <v>55</v>
       </c>
-      <c r="X10" s="14">
+      <c r="X10" s="11">
         <v>46018</v>
       </c>
-      <c r="Y10" s="9" t="s">
+      <c r="Y10" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" ht="15.6">
       <c r="A11" s="3">
         <v>45999</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="7">
         <v>6</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18" t="s">
+      <c r="G11" s="18"/>
+      <c r="H11" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="X11" s="14">
+      <c r="X11" s="11">
         <v>46019</v>
       </c>
-      <c r="Y11" s="9" t="s">
+      <c r="Y11" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="15.6">
       <c r="A12" s="3">
         <v>46000</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="7">
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="19"/>
-    </row>
-    <row r="13" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G12" s="18"/>
+      <c r="H12" s="22"/>
+      <c r="X12" s="11">
+        <v>46025</v>
+      </c>
+      <c r="Y12" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="15.6">
       <c r="A13" s="3">
         <v>46001</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="7">
         <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="11" t="s">
+      <c r="E13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="19"/>
-    </row>
-    <row r="14" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H13" s="22"/>
+      <c r="X13" s="11">
+        <v>46026</v>
+      </c>
+      <c r="Y13" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="15.6">
       <c r="A14" s="3">
         <v>46002</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="7">
         <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="19"/>
-    </row>
-    <row r="15" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G14" s="18"/>
+      <c r="H14" s="22"/>
+    </row>
+    <row r="15" spans="1:29" ht="15.6">
       <c r="A15" s="3">
         <v>46003</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="7">
         <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="17"/>
-      <c r="H15" s="19"/>
-    </row>
-    <row r="16" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G15" s="18"/>
+      <c r="H15" s="22"/>
+    </row>
+    <row r="16" spans="1:29" ht="15.6">
       <c r="A16" s="3">
         <v>46004</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.6">
       <c r="A17" s="3">
         <v>46005</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B18" s="8"/>
-      <c r="C18" s="12" t="s">
+      <c r="B17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" spans="1:8" ht="18">
+      <c r="A18" s="13"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D18" s="12"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.6">
       <c r="A19" s="3">
         <v>46006</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="7">
         <v>11</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="17"/>
-      <c r="H19" s="18" t="s">
+      <c r="G19" s="18"/>
+      <c r="H19" s="21" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="15.6">
       <c r="A20" s="3">
         <v>46007</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="7">
         <v>12</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="19"/>
-    </row>
-    <row r="21" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G20" s="18"/>
+      <c r="H20" s="22"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.6">
       <c r="A21" s="3">
         <v>46008</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="7">
         <v>13</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="19"/>
-    </row>
-    <row r="22" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H21" s="22"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.6">
       <c r="A22" s="3">
         <v>46009</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="7">
         <v>14</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G22" s="17" t="s">
+      <c r="G22" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="19"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H22" s="22"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.6">
       <c r="A23" s="3">
         <v>46010</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="7">
         <v>15</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="19"/>
-    </row>
-    <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G23" s="18"/>
+      <c r="H23" s="22"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.6">
       <c r="A24" s="3">
         <v>46011</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.6">
       <c r="A25" s="3">
         <v>46012</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="C26" s="12" t="s">
+      <c r="D25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="1:8" ht="18">
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="9" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.6">
       <c r="A27" s="3">
         <v>46013</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="7">
         <v>16</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="13" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G27" s="18"/>
+      <c r="H27" s="24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.6">
       <c r="A28" s="3">
         <v>46014</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B28" s="7">
         <v>17</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="16" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F28" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" s="18"/>
+      <c r="H28" s="25"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.6">
       <c r="A29" s="3">
         <v>46015</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="7">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H29" s="25"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.6">
       <c r="A30" s="3">
         <v>46016</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="9" t="s">
+      <c r="B30" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="7" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E30" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="13"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="25"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.6">
       <c r="A31" s="3">
         <v>46017</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="7">
         <v>19</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="9"/>
-    </row>
-    <row r="32" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C31" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" s="18"/>
+      <c r="H31" s="25"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.6">
       <c r="A32" s="3">
         <v>46018</v>
       </c>
-      <c r="B32" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B32" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.6">
       <c r="A33" s="3">
         <v>46019</v>
       </c>
-      <c r="B33" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="C34" s="12" t="s">
+      <c r="B33" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+    </row>
+    <row r="34" spans="1:8" ht="18">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="21"/>
-    </row>
-    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D34" s="17"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+    </row>
+    <row r="35" spans="1:8" ht="15.6">
       <c r="A35" s="3">
         <v>46020</v>
       </c>
-      <c r="B35" s="9">
+      <c r="B35" s="7">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C35" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" s="18"/>
+      <c r="H35" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.6">
       <c r="A36" s="3">
         <v>46021</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="12">
         <v>21</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C36" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G36" s="18"/>
+      <c r="H36" s="25"/>
+    </row>
+    <row r="37" spans="1:8" ht="15.6">
       <c r="A37" s="3">
         <v>46022</v>
       </c>
-      <c r="B37" s="9">
+      <c r="B37" s="7">
         <v>22</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="E37" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" s="13"/>
+      <c r="G37" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H37" s="25"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.6">
+      <c r="A38" s="3">
+        <v>46023</v>
+      </c>
+      <c r="B38" s="12">
+        <v>23</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="13"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="25"/>
+    </row>
+    <row r="39" spans="1:8" ht="15.6">
+      <c r="A39" s="3">
+        <v>46024</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G39" s="18"/>
+      <c r="H39" s="25"/>
+    </row>
+    <row r="40" spans="1:8" ht="15.6">
+      <c r="A40" s="3">
+        <v>46025</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+    </row>
+    <row r="41" spans="1:8" ht="15.6">
+      <c r="A41" s="3">
+        <v>46026</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+    </row>
+    <row r="42" spans="1:8" ht="18">
+      <c r="C42" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.6">
+      <c r="A43" s="3">
+        <v>46027</v>
+      </c>
+      <c r="B43" s="12">
+        <v>24</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G43" s="18"/>
+      <c r="H43" s="13"/>
+    </row>
+    <row r="44" spans="1:8" ht="15.6">
+      <c r="A44" s="3">
+        <v>46028</v>
+      </c>
+      <c r="B44" s="12">
+        <v>25</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G44" s="18"/>
+    </row>
+    <row r="45" spans="1:8" ht="15.6">
+      <c r="A45" s="3"/>
+      <c r="B45" s="12"/>
+      <c r="G45" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15.6">
+      <c r="A46" s="3"/>
+      <c r="B46" s="12"/>
+      <c r="G46" s="19"/>
+    </row>
+    <row r="47" spans="1:8" ht="15.6">
+      <c r="A47" s="3"/>
+      <c r="B47" s="12"/>
+      <c r="G47" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="22">
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H31"/>
+    <mergeCell ref="G35:G36"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="H19:H23"/>
     <mergeCell ref="G14:G15"/>
@@ -1634,7 +2088,11 @@
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="H3:H7"/>
     <mergeCell ref="H11:H15"/>
-    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H35:H39"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="G30:G31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" tooltip="Day -7 Blog app create popup and animation" display="https://github.com/AakashChidambaranathan/Intership_task/commit/47e9946674f87f428e5d2cff5875e3cca658dd67" xr:uid="{2740968A-86F6-4ABB-8E7C-25250927D97F}"/>
@@ -1655,8 +2113,1274 @@
     <hyperlink ref="E23" r:id="rId16" display="https://github.com/AakashChidambaranathan/Intership_task/tree/8702c10b09067fcb834f14066909a04ddc83680e" xr:uid="{14736496-F2DA-481F-9D9D-5AB3AE7C15C3}"/>
     <hyperlink ref="E27" r:id="rId17" display="https://github.com/AakashChidambaranathan/Intership_task/tree/2385d676f720ebd8a58de01590373056baf3a957" xr:uid="{F0BDF0C3-BC66-4764-9A83-13AAB2D059C6}"/>
     <hyperlink ref="E28" r:id="rId18" display="https://github.com/AakashChidambaranathan/Intership_task/tree/0470b045f604410b0cb1eeecd44a8d810df89475" xr:uid="{53DA9962-094B-4F7E-B20F-CD07E8D4391B}"/>
+    <hyperlink ref="E31" r:id="rId19" display="https://github.com/AakashChidambaranathan/Intership_task/tree/5e82dcb38869f9dae5bf244ad47810f0bde98f7d" xr:uid="{105DC5B2-A679-436E-9382-1050437CEC13}"/>
+    <hyperlink ref="E43" r:id="rId20" display="https://github.com/AakashChidambaranathan/Intership_task/tree/9135683980ad23825bb62e52e371e0f6e3c013c4" xr:uid="{23D49AAF-AEC8-43A9-ABFA-FEF9A4844A33}"/>
+    <hyperlink ref="E29" r:id="rId21" display="https://github.com/AakashChidambaranathan/Intership_task/tree/c0f18dc48dfe3188a657f8099cc04fcddf58a7e0" xr:uid="{F716D4A2-1EFA-4B92-AB41-DF2E6033B38C}"/>
+    <hyperlink ref="E39" r:id="rId22" display="https://github.com/AakashChidambaranathan/Intership_task/tree/c0f18dc48dfe3188a657f8099cc04fcddf58a7e0" xr:uid="{6E53656A-0C82-4E7A-A65A-FDE835A1BA01}"/>
+    <hyperlink ref="E35" r:id="rId23" display="https://github.com/AakashChidambaranathan/Intership_task/tree/5e82dcb38869f9dae5bf244ad47810f0bde98f7d" xr:uid="{78FC8660-1532-4FD2-A5B0-37DF01A54746}"/>
+    <hyperlink ref="E36" r:id="rId24" display="https://github.com/AakashChidambaranathan/Intership_task/tree/5e82dcb38869f9dae5bf244ad47810f0bde98f7d" xr:uid="{0E926C9D-B86F-4B1F-BF51-A7FC0A9B4678}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E3E4F9-9B7C-4166-B756-1C0E93C0BC1D}">
+  <dimension ref="A1:K46"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="73" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="115.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.88671875" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" customWidth="1"/>
+    <col min="6" max="6" width="71.5546875" customWidth="1"/>
+    <col min="7" max="7" width="30.77734375" customWidth="1"/>
+    <col min="8" max="8" width="78.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="17.399999999999999">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" ht="18">
+      <c r="A2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.6">
+      <c r="A3" s="3">
+        <v>45992</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.6">
+      <c r="A4" s="3">
+        <v>45993</v>
+      </c>
+      <c r="B4" s="7">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="23"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.6">
+      <c r="A5" s="3">
+        <v>45994</v>
+      </c>
+      <c r="B5" s="7">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="23"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.6">
+      <c r="A6" s="3">
+        <v>45995</v>
+      </c>
+      <c r="B6" s="7">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="18"/>
+      <c r="H6" s="23"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.6">
+      <c r="A7" s="3">
+        <v>45996</v>
+      </c>
+      <c r="B7" s="7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="23"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.6">
+      <c r="A8" s="3">
+        <v>45997</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.6">
+      <c r="A9" s="3">
+        <v>45998</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="1:8" ht="18">
+      <c r="A10" s="13"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.6">
+      <c r="A11" s="3">
+        <v>45999</v>
+      </c>
+      <c r="B11" s="7">
+        <v>6</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.6">
+      <c r="A12" s="3">
+        <v>46000</v>
+      </c>
+      <c r="B12" s="7">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="18"/>
+      <c r="H12" s="22"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.6">
+      <c r="A13" s="3">
+        <v>46001</v>
+      </c>
+      <c r="B13" s="7">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="22"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.6">
+      <c r="A14" s="3">
+        <v>46002</v>
+      </c>
+      <c r="B14" s="7">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="18"/>
+      <c r="H14" s="22"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.6">
+      <c r="A15" s="3">
+        <v>46003</v>
+      </c>
+      <c r="B15" s="7">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="18"/>
+      <c r="H15" s="22"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.6">
+      <c r="A16" s="3">
+        <v>46004</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.6">
+      <c r="A17" s="3">
+        <v>46005</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" spans="1:11" ht="18">
+      <c r="A18" s="13"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+    </row>
+    <row r="19" spans="1:11" ht="15.6">
+      <c r="A19" s="3">
+        <v>46006</v>
+      </c>
+      <c r="B19" s="7">
+        <v>11</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+    </row>
+    <row r="20" spans="1:11" ht="15.6">
+      <c r="A20" s="3">
+        <v>46007</v>
+      </c>
+      <c r="B20" s="7">
+        <v>12</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="18"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+    </row>
+    <row r="21" spans="1:11" ht="15.6">
+      <c r="A21" s="3">
+        <v>46008</v>
+      </c>
+      <c r="B21" s="7">
+        <v>13</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="30"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+    </row>
+    <row r="22" spans="1:11" ht="15.6">
+      <c r="A22" s="3">
+        <v>46009</v>
+      </c>
+      <c r="B22" s="7">
+        <v>14</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" s="30"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.6">
+      <c r="A23" s="3">
+        <v>46010</v>
+      </c>
+      <c r="B23" s="7">
+        <v>15</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" s="18"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+    </row>
+    <row r="24" spans="1:11" ht="15.6">
+      <c r="A24" s="3">
+        <v>46011</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+    </row>
+    <row r="25" spans="1:11" ht="15.6">
+      <c r="A25" s="3">
+        <v>46012</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+    </row>
+    <row r="26" spans="1:11" ht="18">
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.6">
+      <c r="A27" s="3">
+        <v>46013</v>
+      </c>
+      <c r="B27" s="7">
+        <v>16</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" s="18"/>
+      <c r="H27" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31"/>
+    </row>
+    <row r="28" spans="1:11" ht="15.6">
+      <c r="A28" s="3">
+        <v>46014</v>
+      </c>
+      <c r="B28" s="7">
+        <v>17</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" s="18"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="31"/>
+    </row>
+    <row r="29" spans="1:11" ht="15.6">
+      <c r="A29" s="3">
+        <v>46015</v>
+      </c>
+      <c r="B29" s="7">
+        <v>18</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H29" s="33"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+    </row>
+    <row r="30" spans="1:11" ht="15.6">
+      <c r="A30" s="3">
+        <v>46016</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="13"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+    </row>
+    <row r="31" spans="1:11" ht="15.6">
+      <c r="A31" s="3">
+        <v>46017</v>
+      </c>
+      <c r="B31" s="7">
+        <v>19</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" s="18"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="31"/>
+    </row>
+    <row r="32" spans="1:11" ht="15.6">
+      <c r="A32" s="3">
+        <v>46018</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
+    </row>
+    <row r="33" spans="1:11" ht="15.6">
+      <c r="A33" s="3">
+        <v>46019</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="31"/>
+    </row>
+    <row r="34" spans="1:11" ht="18">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" s="17"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
+    </row>
+    <row r="35" spans="1:11" ht="15.6">
+      <c r="A35" s="3">
+        <v>46020</v>
+      </c>
+      <c r="B35" s="7">
+        <v>20</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" s="18"/>
+      <c r="H35" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+    </row>
+    <row r="36" spans="1:11" ht="15.6">
+      <c r="A36" s="3">
+        <v>46021</v>
+      </c>
+      <c r="B36" s="12">
+        <v>21</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G36" s="18"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+    </row>
+    <row r="37" spans="1:11" ht="15.6">
+      <c r="A37" s="3">
+        <v>46022</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" s="13"/>
+      <c r="G37" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H37" s="33"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
+    </row>
+    <row r="38" spans="1:11" ht="15.6">
+      <c r="A38" s="3"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="31"/>
+    </row>
+    <row r="39" spans="1:11" ht="15.6">
+      <c r="A39" s="3"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
+    </row>
+    <row r="40" spans="1:11" ht="15.6">
+      <c r="H40" s="31"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="31"/>
+    </row>
+    <row r="41" spans="1:11" ht="15.6">
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="31"/>
+    </row>
+    <row r="42" spans="1:11" ht="15.6">
+      <c r="H42" s="31"/>
+      <c r="I42" s="31"/>
+      <c r="J42" s="31"/>
+      <c r="K42" s="31"/>
+    </row>
+    <row r="43" spans="1:11" ht="15.6">
+      <c r="H43" s="31"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="31"/>
+      <c r="K43" s="31"/>
+    </row>
+    <row r="44" spans="1:11" ht="15.6">
+      <c r="H44" s="31"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="31"/>
+      <c r="K44" s="31"/>
+    </row>
+    <row r="45" spans="1:11" ht="15.6">
+      <c r="H45" s="31"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="31"/>
+      <c r="K45" s="31"/>
+    </row>
+    <row r="46" spans="1:11" ht="15.6">
+      <c r="H46" s="31"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
+      <c r="K46" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H31"/>
+    <mergeCell ref="G30:G31"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C11" r:id="rId1" tooltip="Day -7 Blog app create popup and animation" display="https://github.com/AakashChidambaranathan/Intership_task/commit/47e9946674f87f428e5d2cff5875e3cca658dd67" xr:uid="{E6BF1654-2E60-4C7B-8C06-71168BF228BE}"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://github.com/AakashChidambaranathan/Intership_task/tree/b173e2d43ecb1fd92e9d3f8ea145f4a80c1ea62c" xr:uid="{7817A557-9972-4B00-A9CF-D571DBF09257}"/>
+    <hyperlink ref="E4" r:id="rId3" display="https://github.com/AakashChidambaranathan/Intership_task/tree/b173e2d43ecb1fd92e9d3f8ea145f4a80c1ea62c" xr:uid="{2A5F4EF0-760A-4FC7-BC82-32E4BC70B298}"/>
+    <hyperlink ref="E5" r:id="rId4" display="https://github.com/AakashChidambaranathan/Intership_task/tree/492c28a482b2757a441e3dbc986bf024969d1e78" xr:uid="{09DF44CC-C6E2-4FB8-B6CE-DC4C5A2F0D76}"/>
+    <hyperlink ref="E6" r:id="rId5" display="https://github.com/AakashChidambaranathan/Intership_task/tree/4d8e8c4efe1c4d6c2951e9567b5a30fd9753930f" xr:uid="{919655A9-C59C-4E97-AE6D-0A2D9F0048D3}"/>
+    <hyperlink ref="E7" r:id="rId6" display="https://github.com/AakashChidambaranathan/Intership_task/tree/0219356c732cd4e6a9f90160fbb3aa0095e6ad70" xr:uid="{EC35E59E-08B9-4D2A-866E-30368BB6FE3B}"/>
+    <hyperlink ref="E11" r:id="rId7" display="https://github.com/AakashChidambaranathan/Intership_task/tree/fabb22e71f0786d4df5ddba16ff5e56255455d94" xr:uid="{C32B32D7-96DD-4D0E-8230-C1FEEF9213AA}"/>
+    <hyperlink ref="E12" r:id="rId8" display="https://github.com/AakashChidambaranathan/Intership_task/tree/fabb22e71f0786d4df5ddba16ff5e56255455d94" xr:uid="{68F22228-763A-48F7-8FB0-2D0D0C539D46}"/>
+    <hyperlink ref="E14" r:id="rId9" display="https://github.com/AakashChidambaranathan/Intership_task/tree/f8d6a572c3bd2738f9f29acd251ec176e69bb852" xr:uid="{E64FB969-150D-4120-962C-66157ECF7642}"/>
+    <hyperlink ref="E15" r:id="rId10" display="https://github.com/AakashChidambaranathan/Intership_task/tree/99b5f9cb065f0c3226b532596a7ec487a3f9dbcf" xr:uid="{6708C4F8-52B5-4761-8E7D-5AD4959E15F1}"/>
+    <hyperlink ref="E19" r:id="rId11" xr:uid="{198C52AA-4645-440B-A8DA-42C05C1F37C3}"/>
+    <hyperlink ref="E20" r:id="rId12" display="https://github.com/AakashChidambaranathan/Intership_task/tree/f2e646fc76a8ead55f6b5c582100ae58d402bfa0" xr:uid="{70B69D03-62E9-471F-8973-87401A9D849B}"/>
+    <hyperlink ref="C21" r:id="rId13" tooltip="dynamic change text" display="https://github.com/AakashChidambaranathan/Intership_task/commit/b1ca1109002a654f7551b2c3c0e56c48460bf95e" xr:uid="{768B6B18-358A-4CA6-938D-C5DFBFB7EA59}"/>
+    <hyperlink ref="E21" r:id="rId14" xr:uid="{77B79982-F26F-44AB-ADD7-89BEF7579EFC}"/>
+    <hyperlink ref="E22" r:id="rId15" display="https://github.com/AakashChidambaranathan/Intership_task/tree/2dd6098d3b32e05b05fd6d455f18f7de6abae75d" xr:uid="{F107F621-3E70-4812-AC18-7ED8B004756B}"/>
+    <hyperlink ref="E23" r:id="rId16" display="https://github.com/AakashChidambaranathan/Intership_task/tree/8702c10b09067fcb834f14066909a04ddc83680e" xr:uid="{C35F4B2A-38EA-4D35-AFAF-AC6C304DFD4C}"/>
+    <hyperlink ref="E27" r:id="rId17" display="https://github.com/AakashChidambaranathan/Intership_task/tree/2385d676f720ebd8a58de01590373056baf3a957" xr:uid="{B0F3613D-FCC2-4C95-B9C7-FBEB99E4D624}"/>
+    <hyperlink ref="E28" r:id="rId18" display="https://github.com/AakashChidambaranathan/Intership_task/tree/0470b045f604410b0cb1eeecd44a8d810df89475" xr:uid="{80279966-B436-4BE2-A14D-B99C8CE9D3A3}"/>
+    <hyperlink ref="E31" r:id="rId19" display="https://github.com/AakashChidambaranathan/Intership_task/tree/5e82dcb38869f9dae5bf244ad47810f0bde98f7d" xr:uid="{8F0FDFD8-FFEC-45BC-A795-49023EA845D0}"/>
+    <hyperlink ref="E29" r:id="rId20" display="https://github.com/AakashChidambaranathan/Intership_task/tree/c0f18dc48dfe3188a657f8099cc04fcddf58a7e0" xr:uid="{2AB6BC5D-99AA-4CF9-A936-0B92D62C4D6F}"/>
+    <hyperlink ref="E35" r:id="rId21" display="https://github.com/AakashChidambaranathan/Intership_task/tree/5e82dcb38869f9dae5bf244ad47810f0bde98f7d" xr:uid="{0F50DFA5-15B8-47D9-97FD-77C03B64A862}"/>
+    <hyperlink ref="E36" r:id="rId22" display="https://github.com/AakashChidambaranathan/Intership_task/tree/5e82dcb38869f9dae5bf244ad47810f0bde98f7d" xr:uid="{EF5FB746-0C42-4B95-8D0C-46A453AD4159}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E91C5E-F27B-41D1-8BA2-ADBA109D0125}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView zoomScale="124" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="48.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="61.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="144.77734375" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="6" customFormat="1" ht="17.399999999999999">
+      <c r="A1" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="25.8" customHeight="1">
+      <c r="A2" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="43.8" customHeight="1">
+      <c r="A6" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="31.2">
+      <c r="A7" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="28"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" s="28"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067CD26F-59C3-4E64-958A-2E77ABDDEFF2}">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView zoomScale="114" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" customWidth="1"/>
+    <col min="10" max="10" width="21.77734375" customWidth="1"/>
+    <col min="11" max="11" width="26.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="17.399999999999999">
+      <c r="A1" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="6"/>
+      <c r="F1" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="20"/>
+      <c r="J1" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" s="19"/>
+    </row>
+    <row r="2" spans="1:11" ht="17.399999999999999">
+      <c r="A2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="F2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.6">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11">
+        <v>46001</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="11">
+        <v>45997</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="7">
+        <v>25</v>
+      </c>
+      <c r="K3" s="7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.6">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11">
+        <v>46022</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="11">
+        <v>45998</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.6">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11">
+        <v>46023</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="11">
+        <v>46004</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.6">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="F6" s="11">
+        <v>46005</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.6">
+      <c r="F7" s="11">
+        <v>46011</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.6">
+      <c r="F8" s="11">
+        <v>46012</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.6">
+      <c r="F9" s="11">
+        <v>46016</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.6">
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="11">
+        <v>46018</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.6">
+      <c r="F11" s="11">
+        <v>46019</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.6">
+      <c r="F12" s="11">
+        <v>46025</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.6">
+      <c r="F13" s="11">
+        <v>46026</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Blog add and profile page design
</commit_message>
<xml_diff>
--- a/Daliy report for intership.xlsx
+++ b/Daliy report for intership.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\intership\task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9021F2B6-4AB4-495D-AC56-CECCF7A3854B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBD54A9-EA7C-4321-8508-A5DD6513C00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3B151EBB-8F28-4EA9-9DF6-8FD080780458}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="117">
   <si>
     <t>Date</t>
   </si>
@@ -419,26 +419,86 @@
     <t>Notes link(Github)</t>
   </si>
   <si>
-    <t>Cors: https://github.com/AakashChidambaranathan/Intership_task/blob/main/Notes/NodeJs/cors.txt  file_System(method):https://github.com/AakashChidambaranathan/Intership_task/blob/main/Notes/NodeJs/file_System(method).txt</t>
-  </si>
-  <si>
     <t>WORKING DAYS (Upto 06-01-2026)</t>
   </si>
   <si>
     <t>Technology Used</t>
   </si>
   <si>
-    <t>Task Description</t>
-  </si>
-  <si>
     <t>Reference  (GitHub Commit)</t>
+  </si>
+  <si>
+    <r>
+      <t>Task Description (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Blog App Development</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Live Website URL:</t>
+  </si>
+  <si>
+    <t>Project Title:</t>
+  </si>
+  <si>
+    <t>Blog Management Web Application</t>
+  </si>
+  <si>
+    <t>intership-task-eight.vercel.app</t>
+  </si>
+  <si>
+    <r>
+      <t>Task Website</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Live demo link)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Cors: https://github.com/AakashChidambaranathan/Intership_task/blob/main/Notes/NodeJs/cors.txt  </t>
+  </si>
+  <si>
+    <t>file_System(method) :https://github.com/AakashChidambaranathan/Intership_task/blob/main/Notes/NodeJs/file_System(method).txt</t>
+  </si>
+  <si>
+    <t>React and Express(change desing on profile and blog add page also new funcation)</t>
+  </si>
+  <si>
+    <t>React,Express and json</t>
+  </si>
+  <si>
+    <t>AakashChidambaranathan/Intership_task at 18b1e04fd0c68ab22467b44fc88aff51db5fa982</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,6 +565,36 @@
       <color theme="1"/>
       <name val="Times New Roman\"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -533,7 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -566,13 +656,25 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -580,6 +682,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -590,14 +695,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -605,15 +710,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -932,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D999300A-A676-4830-BF8B-3ED0F14791B7}">
   <dimension ref="A1:AC47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="94" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -945,9 +1046,12 @@
     <col min="5" max="5" width="77.88671875" customWidth="1"/>
     <col min="6" max="6" width="50.5546875" customWidth="1"/>
     <col min="7" max="7" width="27.77734375" customWidth="1"/>
-    <col min="8" max="8" width="52.77734375" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="20.109375" customWidth="1"/>
+    <col min="8" max="8" width="65.109375" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="39.6640625" customWidth="1"/>
+    <col min="11" max="11" width="31.44140625" customWidth="1"/>
+    <col min="12" max="12" width="42.44140625" customWidth="1"/>
+    <col min="13" max="13" width="44.6640625" customWidth="1"/>
     <col min="14" max="14" width="53.21875" customWidth="1"/>
     <col min="19" max="19" width="7.88671875" customWidth="1"/>
     <col min="20" max="20" width="12.77734375" customWidth="1"/>
@@ -960,7 +1064,7 @@
     <col min="29" max="29" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="17.399999999999999">
+    <row r="1" spans="1:29" ht="18">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -971,36 +1075,41 @@
         <v>106</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>105</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="M1" s="20" t="s">
+      <c r="H1" s="25"/>
+      <c r="I1" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" s="33"/>
+      <c r="K1" s="23"/>
+      <c r="M1" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="20"/>
-      <c r="S1" s="20" t="s">
+      <c r="N1" s="25"/>
+      <c r="S1" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
       <c r="V1" s="6"/>
-      <c r="X1" s="20" t="s">
+      <c r="X1" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" s="20"/>
-      <c r="AB1" s="20" t="s">
+      <c r="Y1" s="25"/>
+      <c r="AB1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="AC1" s="19"/>
+      <c r="AC1" s="26"/>
     </row>
     <row r="2" spans="1:29" ht="18">
       <c r="A2" s="13"/>
@@ -1013,6 +1122,13 @@
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
+      <c r="I2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K2" s="22"/>
       <c r="M2" s="9" t="s">
         <v>65</v>
       </c>
@@ -1061,10 +1177,17 @@
       <c r="F3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="21" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="27" t="s">
         <v>37</v>
       </c>
+      <c r="I3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K3" s="22"/>
       <c r="M3" s="7" t="s">
         <v>67</v>
       </c>
@@ -1113,8 +1236,10 @@
       <c r="F4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="23"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="22"/>
       <c r="M4" s="7" t="s">
         <v>38</v>
       </c>
@@ -1162,7 +1287,7 @@
       <c r="G5" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="23"/>
+      <c r="H5" s="30"/>
       <c r="M5" s="7" t="s">
         <v>68</v>
       </c>
@@ -1205,8 +1330,8 @@
       <c r="F6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="23"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="30"/>
       <c r="M6" s="7" t="s">
         <v>97</v>
       </c>
@@ -1242,12 +1367,12 @@
       <c r="F7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="23"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="30"/>
       <c r="M7" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="N7" s="27" t="s">
+      <c r="N7" s="18" t="s">
         <v>100</v>
       </c>
       <c r="X7" s="11">
@@ -1257,7 +1382,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:29" ht="17.399999999999999">
+    <row r="8" spans="1:29" ht="15.6">
       <c r="A8" s="3">
         <v>45997</v>
       </c>
@@ -1278,8 +1403,6 @@
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="26"/>
       <c r="X8" s="11">
         <v>46012</v>
       </c>
@@ -1308,7 +1431,6 @@
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
-      <c r="N9" s="26"/>
       <c r="X9" s="11">
         <v>46016</v>
       </c>
@@ -1327,7 +1449,6 @@
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
-      <c r="N10" s="26"/>
       <c r="V10" t="s">
         <v>55</v>
       </c>
@@ -1357,8 +1478,8 @@
       <c r="F11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="21" t="s">
+      <c r="G11" s="29"/>
+      <c r="H11" s="27" t="s">
         <v>39</v>
       </c>
       <c r="X11" s="11">
@@ -1387,8 +1508,8 @@
       <c r="F12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="22"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="28"/>
       <c r="X12" s="11">
         <v>46025</v>
       </c>
@@ -1416,7 +1537,7 @@
       <c r="G13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="22"/>
+      <c r="H13" s="28"/>
       <c r="X13" s="11">
         <v>46026</v>
       </c>
@@ -1443,8 +1564,8 @@
       <c r="F14" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="22"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="28"/>
     </row>
     <row r="15" spans="1:29" ht="15.6">
       <c r="A15" s="3">
@@ -1465,8 +1586,8 @@
       <c r="F15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="22"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="28"/>
     </row>
     <row r="16" spans="1:29" ht="15.6">
       <c r="A16" s="3">
@@ -1490,7 +1611,7 @@
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="1:8" ht="15.6">
+    <row r="17" spans="1:14" ht="15.6">
       <c r="A17" s="3">
         <v>46005</v>
       </c>
@@ -1512,7 +1633,7 @@
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="1:8" ht="18">
+    <row r="18" spans="1:14" ht="18">
       <c r="A18" s="13"/>
       <c r="B18" s="12"/>
       <c r="C18" s="9" t="s">
@@ -1524,7 +1645,7 @@
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="1:8" ht="15.6">
+    <row r="19" spans="1:14" ht="15.6">
       <c r="A19" s="3">
         <v>46006</v>
       </c>
@@ -1543,12 +1664,13 @@
       <c r="F19" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="21" t="s">
+      <c r="G19" s="29"/>
+      <c r="H19" s="27" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.6">
+      <c r="N19" s="21"/>
+    </row>
+    <row r="20" spans="1:14" ht="15.6">
       <c r="A20" s="3">
         <v>46007</v>
       </c>
@@ -1567,10 +1689,11 @@
       <c r="F20" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="22"/>
-    </row>
-    <row r="21" spans="1:8" ht="15.6">
+      <c r="G20" s="29"/>
+      <c r="H20" s="28"/>
+      <c r="N20" s="21"/>
+    </row>
+    <row r="21" spans="1:14" ht="15.6">
       <c r="A21" s="3">
         <v>46008</v>
       </c>
@@ -1592,9 +1715,10 @@
       <c r="G21" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="22"/>
-    </row>
-    <row r="22" spans="1:8" ht="15.6">
+      <c r="H21" s="28"/>
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.6">
       <c r="A22" s="3">
         <v>46009</v>
       </c>
@@ -1613,12 +1737,12 @@
       <c r="F22" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="22"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.6">
+      <c r="H22" s="28"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.6">
       <c r="A23" s="3">
         <v>46010</v>
       </c>
@@ -1637,10 +1761,10 @@
       <c r="F23" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="18"/>
-      <c r="H23" s="22"/>
-    </row>
-    <row r="24" spans="1:8" ht="15.6">
+      <c r="G23" s="29"/>
+      <c r="H23" s="28"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.6">
       <c r="A24" s="3">
         <v>46011</v>
       </c>
@@ -1660,7 +1784,7 @@
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="1:8" ht="15.6">
+    <row r="25" spans="1:14" ht="15.6">
       <c r="A25" s="3">
         <v>46012</v>
       </c>
@@ -1680,7 +1804,7 @@
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="1:8" ht="18">
+    <row r="26" spans="1:14" ht="18">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="9" t="s">
@@ -1692,7 +1816,7 @@
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
     </row>
-    <row r="27" spans="1:8" ht="15.6">
+    <row r="27" spans="1:14" ht="15.6">
       <c r="A27" s="3">
         <v>46013</v>
       </c>
@@ -1711,12 +1835,12 @@
       <c r="F27" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G27" s="18"/>
-      <c r="H27" s="24" t="s">
+      <c r="G27" s="29"/>
+      <c r="H27" s="31" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.6">
+    <row r="28" spans="1:14" ht="15.6">
       <c r="A28" s="3">
         <v>46014</v>
       </c>
@@ -1735,10 +1859,10 @@
       <c r="F28" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="25"/>
-    </row>
-    <row r="29" spans="1:8" ht="15.6">
+      <c r="G28" s="29"/>
+      <c r="H28" s="32"/>
+    </row>
+    <row r="29" spans="1:14" ht="15.6">
       <c r="A29" s="3">
         <v>46015</v>
       </c>
@@ -1760,9 +1884,9 @@
       <c r="G29" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="H29" s="25"/>
-    </row>
-    <row r="30" spans="1:8" ht="15.6">
+      <c r="H29" s="32"/>
+    </row>
+    <row r="30" spans="1:14" ht="15.6">
       <c r="A30" s="3">
         <v>46016</v>
       </c>
@@ -1779,10 +1903,10 @@
         <v>26</v>
       </c>
       <c r="F30" s="13"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="25"/>
-    </row>
-    <row r="31" spans="1:8" ht="15.6">
+      <c r="G30" s="29"/>
+      <c r="H30" s="32"/>
+    </row>
+    <row r="31" spans="1:14" ht="15.6">
       <c r="A31" s="3">
         <v>46017</v>
       </c>
@@ -1801,10 +1925,10 @@
       <c r="F31" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G31" s="18"/>
-      <c r="H31" s="25"/>
-    </row>
-    <row r="32" spans="1:8" ht="15.6">
+      <c r="G31" s="29"/>
+      <c r="H31" s="32"/>
+    </row>
+    <row r="32" spans="1:14" ht="15.6">
       <c r="A32" s="3">
         <v>46018</v>
       </c>
@@ -1875,8 +1999,8 @@
       <c r="F35" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G35" s="18"/>
-      <c r="H35" s="24" t="s">
+      <c r="G35" s="29"/>
+      <c r="H35" s="31" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1899,8 +2023,8 @@
       <c r="F36" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G36" s="18"/>
-      <c r="H36" s="25"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="32"/>
     </row>
     <row r="37" spans="1:8" ht="15.6">
       <c r="A37" s="3">
@@ -1922,7 +2046,7 @@
       <c r="G37" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="H37" s="25"/>
+      <c r="H37" s="32"/>
     </row>
     <row r="38" spans="1:8" ht="15.6">
       <c r="A38" s="3">
@@ -1941,8 +2065,8 @@
         <v>26</v>
       </c>
       <c r="F38" s="13"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="25"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="32"/>
     </row>
     <row r="39" spans="1:8" ht="15.6">
       <c r="A39" s="3">
@@ -1963,8 +2087,8 @@
       <c r="F39" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G39" s="18"/>
-      <c r="H39" s="25"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="32"/>
     </row>
     <row r="40" spans="1:8" ht="15.6">
       <c r="A40" s="3">
@@ -2034,7 +2158,7 @@
       <c r="F43" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G43" s="18"/>
+      <c r="G43" s="29"/>
       <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:8" ht="15.6">
@@ -2050,11 +2174,27 @@
       <c r="D44" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G44" s="18"/>
+      <c r="E44" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G44" s="29"/>
     </row>
     <row r="45" spans="1:8" ht="15.6">
-      <c r="A45" s="3"/>
-      <c r="B45" s="12"/>
+      <c r="A45" s="3">
+        <v>46029</v>
+      </c>
+      <c r="B45" s="12">
+        <v>26</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>115</v>
+      </c>
       <c r="G45" s="8" t="s">
         <v>92</v>
       </c>
@@ -2062,19 +2202,26 @@
     <row r="46" spans="1:8" ht="15.6">
       <c r="A46" s="3"/>
       <c r="B46" s="12"/>
-      <c r="G46" s="19"/>
+      <c r="G46" s="26"/>
     </row>
     <row r="47" spans="1:8" ht="15.6">
       <c r="A47" s="3"/>
       <c r="B47" s="12"/>
-      <c r="G47" s="19"/>
+      <c r="G47" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="23">
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="G30:G31"/>
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="G27:G28"/>
     <mergeCell ref="H27:H31"/>
     <mergeCell ref="G35:G36"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="H11:H15"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H35:H39"/>
+    <mergeCell ref="G43:G44"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="H19:H23"/>
     <mergeCell ref="G14:G15"/>
@@ -2087,12 +2234,6 @@
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="H3:H7"/>
-    <mergeCell ref="H11:H15"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="H35:H39"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="G30:G31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" tooltip="Day -7 Blog app create popup and animation" display="https://github.com/AakashChidambaranathan/Intership_task/commit/47e9946674f87f428e5d2cff5875e3cca658dd67" xr:uid="{2740968A-86F6-4ABB-8E7C-25250927D97F}"/>
@@ -2119,9 +2260,11 @@
     <hyperlink ref="E39" r:id="rId22" display="https://github.com/AakashChidambaranathan/Intership_task/tree/c0f18dc48dfe3188a657f8099cc04fcddf58a7e0" xr:uid="{6E53656A-0C82-4E7A-A65A-FDE835A1BA01}"/>
     <hyperlink ref="E35" r:id="rId23" display="https://github.com/AakashChidambaranathan/Intership_task/tree/5e82dcb38869f9dae5bf244ad47810f0bde98f7d" xr:uid="{78FC8660-1532-4FD2-A5B0-37DF01A54746}"/>
     <hyperlink ref="E36" r:id="rId24" display="https://github.com/AakashChidambaranathan/Intership_task/tree/5e82dcb38869f9dae5bf244ad47810f0bde98f7d" xr:uid="{0E926C9D-B86F-4B1F-BF51-A7FC0A9B4678}"/>
+    <hyperlink ref="J3" r:id="rId25" display="https://intership-task-eight.vercel.app/" xr:uid="{ED2C5028-6AA5-4DC1-ACD2-06746E888AB3}"/>
+    <hyperlink ref="E44" r:id="rId26" display="https://github.com/AakashChidambaranathan/Intership_task/tree/18b1e04fd0c68ab22467b44fc88aff51db5fa982" xr:uid="{9F103402-4E1C-4D23-8A4C-A6C23EA37A7D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId25"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
 
@@ -2129,8 +2272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E3E4F9-9B7C-4166-B756-1C0E93C0BC1D}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="73" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView zoomScale="66" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2164,10 +2307,10 @@
       <c r="F1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="20"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8" ht="18">
       <c r="A2" s="13"/>
@@ -2200,8 +2343,8 @@
       <c r="F3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="21" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="27" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2224,8 +2367,8 @@
       <c r="F4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="23"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="1:8" ht="15.6">
       <c r="A5" s="3">
@@ -2249,7 +2392,7 @@
       <c r="G5" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="23"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="1:8" ht="15.6">
       <c r="A6" s="3">
@@ -2270,8 +2413,8 @@
       <c r="F6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="23"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="30"/>
     </row>
     <row r="7" spans="1:8" ht="15.6">
       <c r="A7" s="3">
@@ -2292,8 +2435,8 @@
       <c r="F7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="23"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="30"/>
     </row>
     <row r="8" spans="1:8" ht="15.6">
       <c r="A8" s="3">
@@ -2370,8 +2513,8 @@
       <c r="F11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="21" t="s">
+      <c r="G11" s="29"/>
+      <c r="H11" s="27" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2394,8 +2537,8 @@
       <c r="F12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="22"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" ht="15.6">
       <c r="A13" s="3">
@@ -2417,7 +2560,7 @@
       <c r="G13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="22"/>
+      <c r="H13" s="28"/>
     </row>
     <row r="14" spans="1:8" ht="15.6">
       <c r="A14" s="3">
@@ -2438,8 +2581,8 @@
       <c r="F14" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="22"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="28"/>
     </row>
     <row r="15" spans="1:8" ht="15.6">
       <c r="A15" s="3">
@@ -2460,8 +2603,8 @@
       <c r="F15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="22"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="28"/>
     </row>
     <row r="16" spans="1:8" ht="15.6">
       <c r="A16" s="3">
@@ -2517,10 +2660,10 @@
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
     </row>
     <row r="19" spans="1:11" ht="15.6">
       <c r="A19" s="3">
@@ -2541,13 +2684,13 @@
       <c r="F19" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="29" t="s">
+      <c r="G19" s="29"/>
+      <c r="H19" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
     </row>
     <row r="20" spans="1:11" ht="15.6">
       <c r="A20" s="3">
@@ -2568,11 +2711,11 @@
       <c r="F20" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
     </row>
     <row r="21" spans="1:11" ht="15.6">
       <c r="A21" s="3">
@@ -2596,10 +2739,10 @@
       <c r="G21" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="30"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
     </row>
     <row r="22" spans="1:11" ht="15.6">
       <c r="A22" s="3">
@@ -2620,13 +2763,13 @@
       <c r="F22" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="30"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
     </row>
     <row r="23" spans="1:11" ht="15.6">
       <c r="A23" s="3">
@@ -2647,11 +2790,11 @@
       <c r="F23" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="18"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
     </row>
     <row r="24" spans="1:11" ht="15.6">
       <c r="A24" s="3">
@@ -2671,10 +2814,10 @@
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
     </row>
     <row r="25" spans="1:11" ht="15.6">
       <c r="A25" s="3">
@@ -2694,10 +2837,10 @@
       </c>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26" spans="1:11" ht="18">
       <c r="A26" s="13"/>
@@ -2709,10 +2852,10 @@
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
     </row>
     <row r="27" spans="1:11" ht="15.6">
       <c r="A27" s="3">
@@ -2733,13 +2876,13 @@
       <c r="F27" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G27" s="18"/>
-      <c r="H27" s="32" t="s">
+      <c r="G27" s="29"/>
+      <c r="H27" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
     </row>
     <row r="28" spans="1:11" ht="15.6">
       <c r="A28" s="3">
@@ -2760,11 +2903,11 @@
       <c r="F28" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
     </row>
     <row r="29" spans="1:11" ht="15.6">
       <c r="A29" s="3">
@@ -2788,10 +2931,10 @@
       <c r="G29" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="H29" s="33"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
     </row>
     <row r="30" spans="1:11" ht="15.6">
       <c r="A30" s="3">
@@ -2810,11 +2953,11 @@
         <v>26</v>
       </c>
       <c r="F30" s="13"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
     </row>
     <row r="31" spans="1:11" ht="15.6">
       <c r="A31" s="3">
@@ -2835,11 +2978,11 @@
       <c r="F31" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G31" s="18"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
     </row>
     <row r="32" spans="1:11" ht="15.6">
       <c r="A32" s="3">
@@ -2859,10 +3002,10 @@
       </c>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
     </row>
     <row r="33" spans="1:11" ht="15.6">
       <c r="A33" s="3">
@@ -2882,10 +3025,10 @@
       </c>
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
     </row>
     <row r="34" spans="1:11" ht="18">
       <c r="A34" s="13"/>
@@ -2897,10 +3040,10 @@
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
     </row>
     <row r="35" spans="1:11" ht="15.6">
       <c r="A35" s="3">
@@ -2921,13 +3064,13 @@
       <c r="F35" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G35" s="18"/>
-      <c r="H35" s="32" t="s">
+      <c r="G35" s="29"/>
+      <c r="H35" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
     </row>
     <row r="36" spans="1:11" ht="15.6">
       <c r="A36" s="3">
@@ -2948,11 +3091,11 @@
       <c r="F36" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G36" s="18"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
     </row>
     <row r="37" spans="1:11" ht="15.6">
       <c r="A37" s="3">
@@ -2974,10 +3117,10 @@
       <c r="G37" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="H37" s="33"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="31"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
     </row>
     <row r="38" spans="1:11" ht="15.6">
       <c r="A38" s="3"/>
@@ -2986,11 +3129,11 @@
       <c r="D38" s="12"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="31"/>
-      <c r="J38" s="31"/>
-      <c r="K38" s="31"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
     </row>
     <row r="39" spans="1:11" ht="15.6">
       <c r="A39" s="3"/>
@@ -2999,63 +3142,56 @@
       <c r="D39" s="7"/>
       <c r="E39" s="1"/>
       <c r="F39" s="13"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="31"/>
-      <c r="K39" s="31"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
     </row>
     <row r="40" spans="1:11" ht="15.6">
-      <c r="H40" s="31"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
-      <c r="K40" s="31"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
     </row>
     <row r="41" spans="1:11" ht="15.6">
-      <c r="H41" s="31"/>
-      <c r="I41" s="31"/>
-      <c r="J41" s="31"/>
-      <c r="K41" s="31"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
     </row>
     <row r="42" spans="1:11" ht="15.6">
-      <c r="H42" s="31"/>
-      <c r="I42" s="31"/>
-      <c r="J42" s="31"/>
-      <c r="K42" s="31"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
     </row>
     <row r="43" spans="1:11" ht="15.6">
-      <c r="H43" s="31"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="31"/>
-      <c r="K43" s="31"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
     </row>
     <row r="44" spans="1:11" ht="15.6">
-      <c r="H44" s="31"/>
-      <c r="I44" s="31"/>
-      <c r="J44" s="31"/>
-      <c r="K44" s="31"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
     </row>
     <row r="45" spans="1:11" ht="15.6">
-      <c r="H45" s="31"/>
-      <c r="I45" s="31"/>
-      <c r="J45" s="31"/>
-      <c r="K45" s="31"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
     </row>
     <row r="46" spans="1:11" ht="15.6">
-      <c r="H46" s="31"/>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
-      <c r="K46" s="31"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H15"/>
-    <mergeCell ref="G14:G15"/>
     <mergeCell ref="G35:G36"/>
     <mergeCell ref="H35:H39"/>
     <mergeCell ref="G38:G39"/>
@@ -3065,6 +3201,13 @@
     <mergeCell ref="G27:G28"/>
     <mergeCell ref="H27:H31"/>
     <mergeCell ref="G30:G31"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H15"/>
+    <mergeCell ref="G14:G15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" tooltip="Day -7 Blog app create popup and animation" display="https://github.com/AakashChidambaranathan/Intership_task/commit/47e9946674f87f428e5d2cff5875e3cca658dd67" xr:uid="{E6BF1654-2E60-4C7B-8C06-71168BF228BE}"/>
@@ -3098,8 +3241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E91C5E-F27B-41D1-8BA2-ADBA109D0125}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScale="124" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="70" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -3110,14 +3253,12 @@
     <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="17.399999999999999">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:3" s="24" customFormat="1" ht="22.8">
+      <c r="A1" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="9" t="s">
-        <v>102</v>
-      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
     </row>
     <row r="2" spans="1:3" ht="25.8" customHeight="1">
       <c r="A2" s="8" t="s">
@@ -3126,7 +3267,9 @@
       <c r="B2" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="9" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
@@ -3152,38 +3295,43 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="43.8" customHeight="1">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:3" ht="22.2" customHeight="1">
+      <c r="A6" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="34" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="31.2">
-      <c r="A7" s="7" t="s">
+      <c r="C6" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="31.2">
+      <c r="A8" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B8" s="18" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="28"/>
-    </row>
     <row r="9" spans="1:3">
-      <c r="B9" s="28"/>
+      <c r="B9" s="19"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="B10" s="28"/>
+      <c r="B10" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+  <mergeCells count="3">
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3193,8 +3341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067CD26F-59C3-4E64-958A-2E77ABDDEFF2}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView zoomScale="114" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView zoomScale="92" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3208,20 +3356,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.399999999999999">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
       <c r="D1" s="6"/>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="J1" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="K1" s="19"/>
+      <c r="G1" s="25"/>
+      <c r="J1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" s="26"/>
     </row>
     <row r="2" spans="1:11" ht="17.399999999999999">
       <c r="A2" s="8" t="s">

</xml_diff>

<commit_message>
change UI on Blog_add page and profile page
</commit_message>
<xml_diff>
--- a/Daliy report for intership.xlsx
+++ b/Daliy report for intership.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\intership\task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7055AA-B8EA-40A1-A0F3-96F4FD8E64EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8934ACC-44BB-49C3-91B3-5238502EA96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3B151EBB-8F28-4EA9-9DF6-8FD080780458}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{3B151EBB-8F28-4EA9-9DF6-8FD080780458}"/>
   </bookViews>
   <sheets>
     <sheet name="Full report" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="126">
   <si>
     <t>Date</t>
   </si>
@@ -495,6 +495,32 @@
   </si>
   <si>
     <t>AakashChidambaranathan/Intership_task at b84f0708446aca28c8dd19967af2615d517a27a7</t>
+  </si>
+  <si>
+    <t>React and Express(Add new funcation)</t>
+  </si>
+  <si>
+    <t>Mysql connection · AakashChidambaranathan/Intership_task@d67f0f0</t>
+  </si>
+  <si>
+    <t>React,Express json and mysql</t>
+  </si>
+  <si>
+    <t>D:\intership\task\Week Six</t>
+  </si>
+  <si>
+    <t>React and Express(Add new funcation and mysql function)-work from home</t>
+  </si>
+  <si>
+    <t>During Week 6, I worked on React and Node.js, focusing on Express with JSON for file operations and data handling.
+I updated the profile and blog pages, improved designs, and added multiple new features.
+The week ended with work-from-home tasks, integrating MySQL operations into the project.</t>
+  </si>
+  <si>
+    <t>week 6</t>
+  </si>
+  <si>
+    <t>MySql connection</t>
   </si>
 </sst>
 </file>
@@ -626,7 +652,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -718,6 +744,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1036,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D999300A-A676-4830-BF8B-3ED0F14791B7}">
   <dimension ref="A1:AC47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" zoomScale="94" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView topLeftCell="A18" zoomScale="69" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1406,6 +1435,12 @@
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
+      <c r="M8" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="X8" s="11">
         <v>46012</v>
       </c>
@@ -2162,7 +2197,9 @@
         <v>45</v>
       </c>
       <c r="G43" s="26"/>
-      <c r="H43" s="13"/>
+      <c r="H43" s="40" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="44" spans="1:8" ht="15.6">
       <c r="A44" s="3">
@@ -2184,6 +2221,7 @@
         <v>45</v>
       </c>
       <c r="G44" s="26"/>
+      <c r="H44" s="33"/>
     </row>
     <row r="45" spans="1:8" ht="15.6">
       <c r="A45" s="3">
@@ -2207,19 +2245,54 @@
       <c r="G45" s="8" t="s">
         <v>92</v>
       </c>
+      <c r="H45" s="33"/>
     </row>
     <row r="46" spans="1:8" ht="15.6">
-      <c r="A46" s="3"/>
-      <c r="B46" s="12"/>
+      <c r="A46" s="3">
+        <v>46030</v>
+      </c>
+      <c r="B46" s="12">
+        <v>27</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>121</v>
+      </c>
       <c r="G46" s="25"/>
+      <c r="H46" s="33"/>
     </row>
     <row r="47" spans="1:8" ht="15.6">
-      <c r="A47" s="3"/>
-      <c r="B47" s="12"/>
+      <c r="A47" s="3">
+        <v>46031</v>
+      </c>
+      <c r="B47" s="12">
+        <v>28</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F47" t="s">
+        <v>121</v>
+      </c>
       <c r="G47" s="25"/>
+      <c r="H47" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="24">
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="H19:H23"/>
     <mergeCell ref="G14:G15"/>
@@ -2243,6 +2316,7 @@
     <mergeCell ref="G38:G39"/>
     <mergeCell ref="H35:H39"/>
     <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H47"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" tooltip="Day -7 Blog app create popup and animation" display="https://github.com/AakashChidambaranathan/Intership_task/commit/47e9946674f87f428e5d2cff5875e3cca658dd67" xr:uid="{2740968A-86F6-4ABB-8E7C-25250927D97F}"/>
@@ -2272,9 +2346,11 @@
     <hyperlink ref="J3" r:id="rId25" display="https://intership-task-eight.vercel.app/" xr:uid="{ED2C5028-6AA5-4DC1-ACD2-06746E888AB3}"/>
     <hyperlink ref="E44" r:id="rId26" display="https://github.com/AakashChidambaranathan/Intership_task/tree/18b1e04fd0c68ab22467b44fc88aff51db5fa982" xr:uid="{9F103402-4E1C-4D23-8A4C-A6C23EA37A7D}"/>
     <hyperlink ref="E45" r:id="rId27" display="https://github.com/AakashChidambaranathan/Intership_task/tree/b84f0708446aca28c8dd19967af2615d517a27a7" xr:uid="{7C7CD810-0E0D-4D05-9C8B-2B100451D532}"/>
+    <hyperlink ref="E46" r:id="rId28" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{411883BD-24F7-40E0-8D73-1D04F1D259BA}"/>
+    <hyperlink ref="E47" r:id="rId29" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{A86CDAB7-7F83-4752-A8E1-29F487667D6B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId28"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
 
@@ -3251,8 +3327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E91C5E-F27B-41D1-8BA2-ADBA109D0125}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScale="70" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -3352,7 +3428,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView zoomScale="92" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3422,10 +3498,10 @@
         <v>50</v>
       </c>
       <c r="J3" s="7">
+        <v>28</v>
+      </c>
+      <c r="K3" s="7">
         <v>25</v>
-      </c>
-      <c r="K3" s="7">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.6">

</xml_diff>

<commit_message>
Create chart using user input
</commit_message>
<xml_diff>
--- a/Daliy report for intership.xlsx
+++ b/Daliy report for intership.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\intership\task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2692F5-2733-448F-B951-03CB44A12CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5361AB-FD37-4B07-A661-AFF682D51AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3B151EBB-8F28-4EA9-9DF6-8FD080780458}"/>
   </bookViews>
   <sheets>
     <sheet name="Full report" sheetId="1" r:id="rId1"/>
-    <sheet name="d" sheetId="5" r:id="rId2"/>
+    <sheet name="January" sheetId="5" r:id="rId2"/>
     <sheet name="December " sheetId="2" r:id="rId3"/>
     <sheet name="Weekly Learning" sheetId="4" r:id="rId4"/>
     <sheet name="Attentancs" sheetId="3" r:id="rId5"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="163">
   <si>
     <t>Date</t>
   </si>
@@ -633,6 +633,50 @@
   </si>
   <si>
     <t>Enhanced the home page, profile page, and job application features using React and Node.js. Improved overall application structure, finalized updates, and documented the work on the report day.</t>
+  </si>
+  <si>
+    <t>D:\intership\task\week_7</t>
+  </si>
+  <si>
+    <t>D:\intership\task\week_8</t>
+  </si>
+  <si>
+    <t>D:\intership\task\week_9</t>
+  </si>
+  <si>
+    <t>week 7</t>
+  </si>
+  <si>
+    <t>week 8</t>
+  </si>
+  <si>
+    <t>week 9</t>
+  </si>
+  <si>
+    <t>week 10</t>
+  </si>
+  <si>
+    <t>week 11</t>
+  </si>
+  <si>
+    <t>React,Node And Mysql</t>
+  </si>
+  <si>
+    <t>Node js  And React</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WEEK 10 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(REACT AND REACT CHARTS)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -764,7 +808,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -815,23 +859,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -842,8 +883,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -862,6 +906,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1178,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D999300A-A676-4830-BF8B-3ED0F14791B7}">
-  <dimension ref="A1:AC73"/>
+  <dimension ref="A1:AC79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="96" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="105" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C69" activeCellId="1" sqref="C74 C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1230,33 +1277,33 @@
       <c r="F1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="34" t="s">
+      <c r="H1" s="30"/>
+      <c r="I1" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="J1" s="34"/>
+      <c r="J1" s="33"/>
       <c r="K1" s="23"/>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="26"/>
-      <c r="S1" s="26" t="s">
+      <c r="N1" s="30"/>
+      <c r="S1" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
       <c r="V1" s="6"/>
-      <c r="X1" s="26" t="s">
+      <c r="X1" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" s="26"/>
-      <c r="AB1" s="26" t="s">
+      <c r="Y1" s="30"/>
+      <c r="AB1" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="AC1" s="27"/>
+      <c r="AC1" s="28"/>
     </row>
     <row r="2" spans="1:29" ht="18">
       <c r="A2" s="13"/>
@@ -1324,8 +1371,8 @@
       <c r="F3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="28" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="34" t="s">
         <v>37</v>
       </c>
       <c r="I3" t="s">
@@ -1383,8 +1430,8 @@
       <c r="F4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="27"/>
       <c r="J4" s="1"/>
       <c r="K4" s="22"/>
       <c r="M4" s="7" t="s">
@@ -1434,7 +1481,7 @@
       <c r="G5" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="31"/>
+      <c r="H5" s="27"/>
       <c r="M5" s="7" t="s">
         <v>68</v>
       </c>
@@ -1477,8 +1524,8 @@
       <c r="F6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="27"/>
       <c r="M6" s="7" t="s">
         <v>97</v>
       </c>
@@ -1514,8 +1561,8 @@
       <c r="F7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="27"/>
       <c r="M7" s="7" t="s">
         <v>98</v>
       </c>
@@ -1584,6 +1631,12 @@
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
+      <c r="M9" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>160</v>
+      </c>
       <c r="X9" s="11">
         <v>46016</v>
       </c>
@@ -1602,6 +1655,12 @@
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
+      <c r="M10" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>145</v>
+      </c>
       <c r="V10" t="s">
         <v>55</v>
       </c>
@@ -1631,9 +1690,15 @@
       <c r="F11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="28" t="s">
+      <c r="G11" s="29"/>
+      <c r="H11" s="34" t="s">
         <v>39</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>161</v>
       </c>
       <c r="X11" s="11">
         <v>46019</v>
@@ -1661,8 +1726,11 @@
       <c r="F12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="30"/>
-      <c r="H12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="35"/>
+      <c r="M12" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="X12" s="11">
         <v>46025</v>
       </c>
@@ -1690,7 +1758,10 @@
       <c r="G13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="29"/>
+      <c r="H13" s="35"/>
+      <c r="M13" s="7" t="s">
+        <v>159</v>
+      </c>
       <c r="X13" s="11">
         <v>46026</v>
       </c>
@@ -1717,8 +1788,8 @@
       <c r="F14" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="1:29" ht="15.6">
       <c r="A15" s="3">
@@ -1739,8 +1810,8 @@
       <c r="F15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="35"/>
     </row>
     <row r="16" spans="1:29" ht="15.6">
       <c r="A16" s="3">
@@ -1817,8 +1888,8 @@
       <c r="F19" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="30"/>
-      <c r="H19" s="28" t="s">
+      <c r="G19" s="29"/>
+      <c r="H19" s="34" t="s">
         <v>74</v>
       </c>
       <c r="N19" s="21"/>
@@ -1842,8 +1913,8 @@
       <c r="F20" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="30"/>
-      <c r="H20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="35"/>
       <c r="N20" s="21"/>
     </row>
     <row r="21" spans="1:14" ht="15.6">
@@ -1868,7 +1939,7 @@
       <c r="G21" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="29"/>
+      <c r="H21" s="35"/>
       <c r="N21" s="1"/>
     </row>
     <row r="22" spans="1:14" ht="15.6">
@@ -1890,10 +1961,10 @@
       <c r="F22" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G22" s="30" t="s">
+      <c r="G22" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="29"/>
+      <c r="H22" s="35"/>
     </row>
     <row r="23" spans="1:14" ht="15.6">
       <c r="A23" s="3">
@@ -1914,8 +1985,8 @@
       <c r="F23" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="30"/>
-      <c r="H23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="35"/>
     </row>
     <row r="24" spans="1:14" ht="15.6">
       <c r="A24" s="3">
@@ -1988,8 +2059,8 @@
       <c r="F27" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G27" s="30"/>
-      <c r="H27" s="32" t="s">
+      <c r="G27" s="29"/>
+      <c r="H27" s="31" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2012,8 +2083,8 @@
       <c r="F28" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G28" s="30"/>
-      <c r="H28" s="33"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="32"/>
     </row>
     <row r="29" spans="1:14" ht="15.6">
       <c r="A29" s="3">
@@ -2037,7 +2108,7 @@
       <c r="G29" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="H29" s="33"/>
+      <c r="H29" s="32"/>
     </row>
     <row r="30" spans="1:14" ht="15.6">
       <c r="A30" s="3">
@@ -2056,8 +2127,8 @@
         <v>26</v>
       </c>
       <c r="F30" s="13"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="33"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="32"/>
     </row>
     <row r="31" spans="1:14" ht="15.6">
       <c r="A31" s="3">
@@ -2078,8 +2149,8 @@
       <c r="F31" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G31" s="30"/>
-      <c r="H31" s="33"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="32"/>
     </row>
     <row r="32" spans="1:14" ht="15.6">
       <c r="A32" s="3">
@@ -2152,8 +2223,8 @@
       <c r="F35" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G35" s="30"/>
-      <c r="H35" s="32" t="s">
+      <c r="G35" s="29"/>
+      <c r="H35" s="31" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2176,8 +2247,8 @@
       <c r="F36" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G36" s="30"/>
-      <c r="H36" s="33"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="32"/>
     </row>
     <row r="37" spans="1:8" ht="15.6">
       <c r="A37" s="3">
@@ -2199,7 +2270,7 @@
       <c r="G37" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="H37" s="33"/>
+      <c r="H37" s="32"/>
     </row>
     <row r="38" spans="1:8" ht="15.6">
       <c r="A38" s="3">
@@ -2218,8 +2289,8 @@
         <v>26</v>
       </c>
       <c r="F38" s="13"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="33"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="32"/>
     </row>
     <row r="39" spans="1:8" ht="15.6">
       <c r="A39" s="3">
@@ -2240,8 +2311,8 @@
       <c r="F39" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G39" s="30"/>
-      <c r="H39" s="33"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="32"/>
     </row>
     <row r="40" spans="1:8" ht="15.6">
       <c r="A40" s="3">
@@ -2312,8 +2383,8 @@
       <c r="F43" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G43" s="30"/>
-      <c r="H43" s="35" t="s">
+      <c r="G43" s="29"/>
+      <c r="H43" s="26" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2336,8 +2407,8 @@
       <c r="F44" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G44" s="30"/>
-      <c r="H44" s="31"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="27"/>
     </row>
     <row r="45" spans="1:8" ht="15.6">
       <c r="A45" s="3">
@@ -2361,7 +2432,7 @@
       <c r="G45" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="H45" s="31"/>
+      <c r="H45" s="27"/>
     </row>
     <row r="46" spans="1:8" ht="15.6">
       <c r="A46" s="3">
@@ -2382,8 +2453,8 @@
       <c r="F46" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="G46" s="27"/>
-      <c r="H46" s="31"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="27"/>
     </row>
     <row r="47" spans="1:8" ht="15.6">
       <c r="A47" s="3">
@@ -2404,8 +2475,8 @@
       <c r="F47" t="s">
         <v>121</v>
       </c>
-      <c r="G47" s="27"/>
-      <c r="H47" s="31"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="27"/>
     </row>
     <row r="48" spans="1:8" ht="15.6">
       <c r="A48" s="3">
@@ -2463,7 +2534,10 @@
       <c r="E51" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="H51" s="35" t="s">
+      <c r="F51" t="s">
+        <v>152</v>
+      </c>
+      <c r="H51" s="26" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2483,7 +2557,10 @@
       <c r="E52" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="H52" s="31"/>
+      <c r="F52" t="s">
+        <v>152</v>
+      </c>
+      <c r="H52" s="27"/>
     </row>
     <row r="53" spans="1:8" ht="15.6">
       <c r="A53" s="3">
@@ -2501,10 +2578,13 @@
       <c r="E53" s="1" t="s">
         <v>119</v>
       </c>
+      <c r="F53" t="s">
+        <v>152</v>
+      </c>
       <c r="G53" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="H53" s="31"/>
+      <c r="H53" s="27"/>
     </row>
     <row r="54" spans="1:8" ht="15.6">
       <c r="A54" s="3">
@@ -2515,7 +2595,10 @@
         <v>6</v>
       </c>
       <c r="D54" s="25"/>
-      <c r="H54" s="31"/>
+      <c r="F54" t="s">
+        <v>152</v>
+      </c>
+      <c r="H54" s="27"/>
     </row>
     <row r="55" spans="1:8" ht="15.6">
       <c r="A55" s="3">
@@ -2531,7 +2614,10 @@
       <c r="E55" t="s">
         <v>119</v>
       </c>
-      <c r="H55" s="31"/>
+      <c r="F55" t="s">
+        <v>152</v>
+      </c>
+      <c r="H55" s="27"/>
     </row>
     <row r="56" spans="1:8" ht="15.6">
       <c r="A56" s="3">
@@ -2576,7 +2662,10 @@
       <c r="E59" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="H59" s="35" t="s">
+      <c r="F59" t="s">
+        <v>153</v>
+      </c>
+      <c r="H59" s="26" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2596,7 +2685,10 @@
       <c r="E60" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="H60" s="35"/>
+      <c r="F60" t="s">
+        <v>153</v>
+      </c>
+      <c r="H60" s="26"/>
     </row>
     <row r="61" spans="1:8" ht="15.6">
       <c r="A61" s="3">
@@ -2609,15 +2701,18 @@
         <v>131</v>
       </c>
       <c r="D61" s="25" t="s">
-        <v>60</v>
+        <v>145</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>138</v>
       </c>
+      <c r="F61" t="s">
+        <v>153</v>
+      </c>
       <c r="G61" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="H61" s="35"/>
+      <c r="H61" s="26"/>
     </row>
     <row r="62" spans="1:8" ht="15.6">
       <c r="A62" s="3">
@@ -2635,7 +2730,10 @@
       <c r="E62" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H62" s="35"/>
+      <c r="F62" t="s">
+        <v>153</v>
+      </c>
+      <c r="H62" s="26"/>
     </row>
     <row r="63" spans="1:8" ht="15.6">
       <c r="A63" s="3">
@@ -2650,7 +2748,7 @@
       <c r="D63" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="H63" s="35"/>
+      <c r="H63" s="26"/>
     </row>
     <row r="64" spans="1:8" ht="15.6">
       <c r="A64" s="3">
@@ -2699,7 +2797,10 @@
       <c r="E67" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="H67" s="27" t="s">
+      <c r="F67" t="s">
+        <v>154</v>
+      </c>
+      <c r="H67" s="42" t="s">
         <v>151</v>
       </c>
     </row>
@@ -2719,7 +2820,10 @@
       <c r="E68" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="H68" s="27"/>
+      <c r="F68" t="s">
+        <v>154</v>
+      </c>
+      <c r="H68" s="42"/>
     </row>
     <row r="69" spans="1:8" ht="15.6">
       <c r="A69" s="3">
@@ -2737,10 +2841,13 @@
       <c r="E69" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="F69" t="s">
+        <v>154</v>
+      </c>
       <c r="G69" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="H69" s="27"/>
+      <c r="H69" s="42"/>
     </row>
     <row r="70" spans="1:8" ht="15.6">
       <c r="A70" s="3">
@@ -2758,7 +2865,10 @@
       <c r="E70" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="H70" s="27"/>
+      <c r="F70" t="s">
+        <v>154</v>
+      </c>
+      <c r="H70" s="42"/>
     </row>
     <row r="71" spans="1:8" ht="15.6">
       <c r="A71" s="3">
@@ -2771,7 +2881,7 @@
         <v>144</v>
       </c>
       <c r="D71" s="25"/>
-      <c r="H71" s="27"/>
+      <c r="H71" s="42"/>
     </row>
     <row r="72" spans="1:8" ht="15.6">
       <c r="A72" s="3">
@@ -2785,27 +2895,63 @@
       </c>
       <c r="D72" s="25"/>
     </row>
-    <row r="73" spans="1:8" ht="15.6">
+    <row r="73" spans="1:8" ht="18">
       <c r="A73" s="3"/>
       <c r="B73" s="25"/>
+      <c r="C73" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="15.6">
+      <c r="A74" s="3">
+        <v>46054</v>
+      </c>
+      <c r="B74" s="25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15.6">
+      <c r="A75" s="3">
+        <v>46055</v>
+      </c>
+      <c r="B75" s="25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="15.6">
+      <c r="A76" s="3">
+        <v>46056</v>
+      </c>
+      <c r="B76" s="25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15.6">
+      <c r="A77" s="3">
+        <v>46057</v>
+      </c>
+      <c r="B77" s="25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="15.6">
+      <c r="A78" s="3">
+        <v>46058</v>
+      </c>
+      <c r="B78" s="25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15.6">
+      <c r="A79" s="3">
+        <v>46059</v>
+      </c>
+      <c r="B79" s="25">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="H51:H55"/>
-    <mergeCell ref="H59:H63"/>
-    <mergeCell ref="H67:H71"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="H27:H31"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="H11:H15"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="H35:H39"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H47"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="H19:H23"/>
     <mergeCell ref="G14:G15"/>
@@ -2818,6 +2964,21 @@
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="H3:H7"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H31"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="H11:H15"/>
+    <mergeCell ref="H35:H39"/>
+    <mergeCell ref="H51:H55"/>
+    <mergeCell ref="H59:H63"/>
+    <mergeCell ref="H67:H71"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H47"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" tooltip="Day -7 Blog app create popup and animation" display="https://github.com/AakashChidambaranathan/Intership_task/commit/47e9946674f87f428e5d2cff5875e3cca658dd67" xr:uid="{2740968A-86F6-4ABB-8E7C-25250927D97F}"/>
@@ -2868,12 +3029,791 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8849BD1A-5B5D-47AB-A398-D3AB96A31B76}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AC39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" zoomScale="70" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" customWidth="1"/>
+    <col min="3" max="3" width="56.109375" customWidth="1"/>
+    <col min="4" max="4" width="57.6640625" customWidth="1"/>
+    <col min="5" max="5" width="37.6640625" customWidth="1"/>
+    <col min="6" max="6" width="45.88671875" customWidth="1"/>
+    <col min="7" max="7" width="33.33203125" customWidth="1"/>
+    <col min="8" max="8" width="36.44140625" customWidth="1"/>
+    <col min="27" max="27" width="13.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" ht="18">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="30"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="23"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="6"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="28"/>
+    </row>
+    <row r="2" spans="1:29" ht="15.6">
+      <c r="A2" s="3">
+        <v>46020</v>
+      </c>
+      <c r="B2" s="7">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="29"/>
+      <c r="H2" s="31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="15.6">
+      <c r="A3" s="3">
+        <v>46021</v>
+      </c>
+      <c r="B3" s="12">
+        <v>21</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="29"/>
+      <c r="H3" s="32"/>
+    </row>
+    <row r="4" spans="1:29" ht="15.6">
+      <c r="A4" s="3">
+        <v>46022</v>
+      </c>
+      <c r="B4" s="7">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="32"/>
+    </row>
+    <row r="5" spans="1:29" ht="15.6">
+      <c r="A5" s="3">
+        <v>46023</v>
+      </c>
+      <c r="B5" s="12">
+        <v>23</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="32"/>
+    </row>
+    <row r="6" spans="1:29" ht="15.6">
+      <c r="A6" s="3">
+        <v>46024</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="29"/>
+      <c r="H6" s="32"/>
+    </row>
+    <row r="7" spans="1:29" ht="15.6">
+      <c r="A7" s="3">
+        <v>46025</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:29" ht="15.6">
+      <c r="A8" s="3">
+        <v>46026</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:29" ht="18">
+      <c r="B9" s="25"/>
+      <c r="C9" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="15.6">
+      <c r="A10" s="3">
+        <v>46027</v>
+      </c>
+      <c r="B10" s="12">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="29"/>
+      <c r="H10" s="26" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="15.6">
+      <c r="A11" s="3">
+        <v>46028</v>
+      </c>
+      <c r="B11" s="12">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="29"/>
+      <c r="H11" s="27"/>
+    </row>
+    <row r="12" spans="1:29" ht="15.6">
+      <c r="A12" s="3">
+        <v>46029</v>
+      </c>
+      <c r="B12" s="12">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="27"/>
+    </row>
+    <row r="13" spans="1:29" ht="15.6">
+      <c r="A13" s="3">
+        <v>46030</v>
+      </c>
+      <c r="B13" s="12">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="G13" s="28"/>
+      <c r="H13" s="27"/>
+    </row>
+    <row r="14" spans="1:29" ht="15.6">
+      <c r="A14" s="3">
+        <v>46031</v>
+      </c>
+      <c r="B14" s="12">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G14" s="28"/>
+      <c r="H14" s="27"/>
+    </row>
+    <row r="15" spans="1:29" ht="15.6">
+      <c r="A15" s="3">
+        <v>46032</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" ht="15.6">
+      <c r="A16" s="3">
+        <v>46033</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="18">
+      <c r="B17" s="25"/>
+      <c r="C17" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.6">
+      <c r="A18" s="3">
+        <v>46034</v>
+      </c>
+      <c r="B18" s="25">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F18" t="s">
+        <v>152</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.6">
+      <c r="A19" s="3">
+        <v>46035</v>
+      </c>
+      <c r="B19" s="25">
+        <v>30</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" t="s">
+        <v>152</v>
+      </c>
+      <c r="H19" s="27"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.6">
+      <c r="A20" s="3">
+        <v>46036</v>
+      </c>
+      <c r="B20" s="25">
+        <v>31</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" t="s">
+        <v>152</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="H20" s="27"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.6">
+      <c r="A21" s="3">
+        <v>46037</v>
+      </c>
+      <c r="B21" s="25"/>
+      <c r="C21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="25"/>
+      <c r="F21" t="s">
+        <v>152</v>
+      </c>
+      <c r="H21" s="27"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.6">
+      <c r="A22" s="3">
+        <v>46038</v>
+      </c>
+      <c r="B22" s="25"/>
+      <c r="C22" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" t="s">
+        <v>119</v>
+      </c>
+      <c r="F22" t="s">
+        <v>152</v>
+      </c>
+      <c r="H22" s="27"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.6">
+      <c r="A23" s="3">
+        <v>46039</v>
+      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="25"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.6">
+      <c r="A24" s="3">
+        <v>46040</v>
+      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="25"/>
+    </row>
+    <row r="25" spans="1:8" ht="18">
+      <c r="B25" s="25"/>
+      <c r="C25" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" s="25"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.6">
+      <c r="A26" s="3">
+        <v>46041</v>
+      </c>
+      <c r="B26" s="25">
+        <v>32</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F26" t="s">
+        <v>153</v>
+      </c>
+      <c r="H26" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.6">
+      <c r="A27" s="3">
+        <v>46042</v>
+      </c>
+      <c r="B27" s="25">
+        <v>33</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F27" t="s">
+        <v>153</v>
+      </c>
+      <c r="H27" s="26"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.6">
+      <c r="A28" s="3">
+        <v>46043</v>
+      </c>
+      <c r="B28" s="25">
+        <v>34</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F28" t="s">
+        <v>153</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="H28" s="26"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.6">
+      <c r="A29" s="3">
+        <v>46044</v>
+      </c>
+      <c r="B29" s="25">
+        <v>35</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F29" t="s">
+        <v>153</v>
+      </c>
+      <c r="H29" s="26"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.6">
+      <c r="A30" s="3">
+        <v>46045</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" s="26"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.6">
+      <c r="A31" s="3">
+        <v>46046</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="25"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.6">
+      <c r="A32" s="3">
+        <v>46047</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="25"/>
+    </row>
+    <row r="33" spans="1:8" ht="18">
+      <c r="B33" s="25"/>
+      <c r="C33" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D33" s="25"/>
+    </row>
+    <row r="34" spans="1:8" ht="15.6">
+      <c r="A34" s="3">
+        <v>46048</v>
+      </c>
+      <c r="B34" s="25">
+        <v>33</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F34" t="s">
+        <v>154</v>
+      </c>
+      <c r="H34" s="42" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.6">
+      <c r="A35" s="3">
+        <v>46049</v>
+      </c>
+      <c r="B35" s="25">
+        <v>34</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F35" t="s">
+        <v>154</v>
+      </c>
+      <c r="H35" s="42"/>
+    </row>
+    <row r="36" spans="1:8" ht="15.6">
+      <c r="A36" s="3">
+        <v>46050</v>
+      </c>
+      <c r="B36" s="25">
+        <v>35</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F36" t="s">
+        <v>154</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="H36" s="42"/>
+    </row>
+    <row r="37" spans="1:8" ht="15.6">
+      <c r="A37" s="3">
+        <v>46051</v>
+      </c>
+      <c r="B37" s="25">
+        <v>36</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F37" t="s">
+        <v>154</v>
+      </c>
+      <c r="H37" s="42"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.6">
+      <c r="A38" s="3">
+        <v>46052</v>
+      </c>
+      <c r="B38" s="25">
+        <v>37</v>
+      </c>
+      <c r="C38" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" s="25"/>
+      <c r="H38" s="42"/>
+    </row>
+    <row r="39" spans="1:8" ht="15.6">
+      <c r="A39" s="3">
+        <v>46053</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="H26:H30"/>
+    <mergeCell ref="H34:H38"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H18:H22"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E10" r:id="rId1" display="https://github.com/AakashChidambaranathan/Intership_task/tree/9135683980ad23825bb62e52e371e0f6e3c013c4" xr:uid="{8318D3D4-2ED6-43C8-BABA-00D454BA9CEC}"/>
+    <hyperlink ref="E6" r:id="rId2" display="https://github.com/AakashChidambaranathan/Intership_task/tree/c0f18dc48dfe3188a657f8099cc04fcddf58a7e0" xr:uid="{CD27853E-FF92-4529-8414-4AC4B1FE09F1}"/>
+    <hyperlink ref="E2" r:id="rId3" display="https://github.com/AakashChidambaranathan/Intership_task/tree/5e82dcb38869f9dae5bf244ad47810f0bde98f7d" xr:uid="{41A44120-6327-4AA9-AA08-1E26904FFB8F}"/>
+    <hyperlink ref="E3" r:id="rId4" display="https://github.com/AakashChidambaranathan/Intership_task/tree/5e82dcb38869f9dae5bf244ad47810f0bde98f7d" xr:uid="{FA38B619-5A4F-4199-ACF1-487F894EA461}"/>
+    <hyperlink ref="E11" r:id="rId5" display="https://github.com/AakashChidambaranathan/Intership_task/tree/18b1e04fd0c68ab22467b44fc88aff51db5fa982" xr:uid="{674501F0-5607-42B0-A077-21C37AEDC1D3}"/>
+    <hyperlink ref="E12" r:id="rId6" display="https://github.com/AakashChidambaranathan/Intership_task/tree/b84f0708446aca28c8dd19967af2615d517a27a7" xr:uid="{CC98102C-0588-4405-8FC2-C208039E9829}"/>
+    <hyperlink ref="E13" r:id="rId7" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{ACCFB52B-8469-4A01-BB12-1072CB2E7D4A}"/>
+    <hyperlink ref="E14" r:id="rId8" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{3401966F-BBC0-4556-A8B2-8BC39D97B489}"/>
+    <hyperlink ref="E18" r:id="rId9" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{7FFE6E63-6412-42E8-9F96-614703015438}"/>
+    <hyperlink ref="E19" r:id="rId10" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{83AB7E3D-3A5E-4FFE-BB5E-9D91C52146E7}"/>
+    <hyperlink ref="E20" r:id="rId11" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{224EF37E-E606-4C2F-AFBD-251FA38DFEA9}"/>
+    <hyperlink ref="E26" r:id="rId12" xr:uid="{77E67683-D0D9-4AA0-B028-6BC935385AF1}"/>
+    <hyperlink ref="E27" r:id="rId13" display="https://github.com/AakashChidambaranathan/Intership_task/tree/2daae779fabe3e1b4a8dbb15b425cf8f38f1447c" xr:uid="{EA1C0276-1B38-4884-B5B2-041BF1C15F2F}"/>
+    <hyperlink ref="E29" r:id="rId14" display="https://github.com/AakashChidambaranathan/Intership_task/tree/ddd3cf7c4973ffcf29e927990c8af509fafabe36" xr:uid="{C245925B-1D76-48C2-ACAD-F70FFF162A80}"/>
+    <hyperlink ref="E28" r:id="rId15" xr:uid="{9AE3D071-6833-4623-94E2-DAEDC1AB9975}"/>
+    <hyperlink ref="E34" r:id="rId16" display="https://github.com/AakashChidambaranathan/Intership_task/tree/bc78e8326ed056418905a04bec214772d22fd6d6" xr:uid="{570ECD13-D24A-4642-B30F-32E14DE13364}"/>
+    <hyperlink ref="E36" r:id="rId17" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d75d5b652c9aa4feb2a5a6e08eceae56ed1d474b" xr:uid="{DC60E8A4-6486-4A12-ACBB-9C7FD4FB4C9B}"/>
+    <hyperlink ref="E35" r:id="rId18" display="https://github.com/AakashChidambaranathan/Intership_task/tree/bc78e8326ed056418905a04bec214772d22fd6d6" xr:uid="{913FA76D-52EB-4FDD-B2B5-2271A634C455}"/>
+    <hyperlink ref="E37" r:id="rId19" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d75d5b652c9aa4feb2a5a6e08eceae56ed1d474b" xr:uid="{E3534CB4-D159-4F79-9E70-E8559F578C8B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2917,10 +3857,10 @@
       <c r="F1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="26"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" ht="18">
       <c r="A2" s="13"/>
@@ -2953,8 +3893,8 @@
       <c r="F3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="28" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="34" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2977,8 +3917,8 @@
       <c r="F4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="27"/>
     </row>
     <row r="5" spans="1:8" ht="15.6">
       <c r="A5" s="3">
@@ -3002,7 +3942,7 @@
       <c r="G5" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="31"/>
+      <c r="H5" s="27"/>
     </row>
     <row r="6" spans="1:8" ht="15.6">
       <c r="A6" s="3">
@@ -3023,8 +3963,8 @@
       <c r="F6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="27"/>
     </row>
     <row r="7" spans="1:8" ht="15.6">
       <c r="A7" s="3">
@@ -3045,8 +3985,8 @@
       <c r="F7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="27"/>
     </row>
     <row r="8" spans="1:8" ht="15.6">
       <c r="A8" s="3">
@@ -3123,8 +4063,8 @@
       <c r="F11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="28" t="s">
+      <c r="G11" s="29"/>
+      <c r="H11" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3147,8 +4087,8 @@
       <c r="F12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="30"/>
-      <c r="H12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:8" ht="15.6">
       <c r="A13" s="3">
@@ -3170,7 +4110,7 @@
       <c r="G13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="29"/>
+      <c r="H13" s="35"/>
     </row>
     <row r="14" spans="1:8" ht="15.6">
       <c r="A14" s="3">
@@ -3191,8 +4131,8 @@
       <c r="F14" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="1:8" ht="15.6">
       <c r="A15" s="3">
@@ -3213,8 +4153,8 @@
       <c r="F15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="35"/>
     </row>
     <row r="16" spans="1:8" ht="15.6">
       <c r="A16" s="3">
@@ -3294,7 +4234,7 @@
       <c r="F19" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="30"/>
+      <c r="G19" s="29"/>
       <c r="H19" s="38" t="s">
         <v>74</v>
       </c>
@@ -3321,7 +4261,7 @@
       <c r="F20" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="30"/>
+      <c r="G20" s="29"/>
       <c r="H20" s="39"/>
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
@@ -3373,7 +4313,7 @@
       <c r="F22" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G22" s="30" t="s">
+      <c r="G22" s="29" t="s">
         <v>55</v>
       </c>
       <c r="H22" s="39"/>
@@ -3400,7 +4340,7 @@
       <c r="F23" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="30"/>
+      <c r="G23" s="29"/>
       <c r="H23" s="39"/>
       <c r="I23" s="20"/>
       <c r="J23" s="20"/>
@@ -3486,7 +4426,7 @@
       <c r="F27" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G27" s="30"/>
+      <c r="G27" s="29"/>
       <c r="H27" s="36" t="s">
         <v>95</v>
       </c>
@@ -3513,7 +4453,7 @@
       <c r="F28" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G28" s="30"/>
+      <c r="G28" s="29"/>
       <c r="H28" s="37"/>
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
@@ -3563,7 +4503,7 @@
         <v>26</v>
       </c>
       <c r="F30" s="13"/>
-      <c r="G30" s="30"/>
+      <c r="G30" s="29"/>
       <c r="H30" s="37"/>
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
@@ -3588,7 +4528,7 @@
       <c r="F31" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G31" s="30"/>
+      <c r="G31" s="29"/>
       <c r="H31" s="37"/>
       <c r="I31" s="20"/>
       <c r="J31" s="20"/>
@@ -3674,7 +4614,7 @@
       <c r="F35" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G35" s="30"/>
+      <c r="G35" s="29"/>
       <c r="H35" s="36" t="s">
         <v>96</v>
       </c>
@@ -3701,7 +4641,7 @@
       <c r="F36" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G36" s="30"/>
+      <c r="G36" s="29"/>
       <c r="H36" s="37"/>
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
@@ -3739,7 +4679,7 @@
       <c r="D38" s="12"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
-      <c r="G38" s="30"/>
+      <c r="G38" s="29"/>
       <c r="H38" s="37"/>
       <c r="I38" s="20"/>
       <c r="J38" s="20"/>
@@ -3752,7 +4692,7 @@
       <c r="D39" s="7"/>
       <c r="E39" s="1"/>
       <c r="F39" s="13"/>
-      <c r="G39" s="30"/>
+      <c r="G39" s="29"/>
       <c r="H39" s="37"/>
       <c r="I39" s="20"/>
       <c r="J39" s="20"/>
@@ -3802,6 +4742,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H15"/>
+    <mergeCell ref="G14:G15"/>
     <mergeCell ref="G35:G36"/>
     <mergeCell ref="H35:H39"/>
     <mergeCell ref="G38:G39"/>
@@ -3811,13 +4758,6 @@
     <mergeCell ref="G27:G28"/>
     <mergeCell ref="H27:H31"/>
     <mergeCell ref="G30:G31"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H15"/>
-    <mergeCell ref="G14:G15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" tooltip="Day -7 Blog app create popup and animation" display="https://github.com/AakashChidambaranathan/Intership_task/commit/47e9946674f87f428e5d2cff5875e3cca658dd67" xr:uid="{E6BF1654-2E60-4C7B-8C06-71168BF228BE}"/>
@@ -3966,20 +4906,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.399999999999999">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
       <c r="D1" s="6"/>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="J1" s="26" t="s">
+      <c r="G1" s="30"/>
+      <c r="J1" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="K1" s="27"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="2" spans="1:11" ht="17.399999999999999">
       <c r="A2" s="8" t="s">

</xml_diff>

<commit_message>
Create otp_login, postmanclone_and_learn redis_db
</commit_message>
<xml_diff>
--- a/Daliy report for intership.xlsx
+++ b/Daliy report for intership.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\intership\task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64318BD1-C537-4BC2-A080-A2C926C3CF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F946453-1AA8-4420-B099-A341D918E9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3B151EBB-8F28-4EA9-9DF6-8FD080780458}"/>
   </bookViews>
   <sheets>
     <sheet name="Full report" sheetId="1" r:id="rId1"/>
-    <sheet name="January" sheetId="5" r:id="rId2"/>
-    <sheet name="December " sheetId="2" r:id="rId3"/>
+    <sheet name="December " sheetId="2" r:id="rId2"/>
+    <sheet name="January" sheetId="5" r:id="rId3"/>
     <sheet name="Weekly Learning" sheetId="4" r:id="rId4"/>
     <sheet name="Attentancs" sheetId="3" r:id="rId5"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="172">
   <si>
     <t>Date</t>
   </si>
@@ -453,33 +453,6 @@
     </r>
   </si>
   <si>
-    <t>Live Website URL:</t>
-  </si>
-  <si>
-    <t>Project Title:</t>
-  </si>
-  <si>
-    <t>Blog Management Web Application</t>
-  </si>
-  <si>
-    <t>intership-task-eight.vercel.app</t>
-  </si>
-  <si>
-    <r>
-      <t>Task Website</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (Live demo link)</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Cors: https://github.com/AakashChidambaranathan/Intership_task/blob/main/Notes/NodeJs/cors.txt  </t>
   </si>
   <si>
@@ -717,12 +690,15 @@
   <si>
     <t>Report Perpation</t>
   </si>
+  <si>
+    <t>holiday(pongal leave)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -799,13 +775,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13.5"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="13.5"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -894,27 +863,24 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -925,11 +891,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -946,7 +915,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1264,10 +1233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D999300A-A676-4830-BF8B-3ED0F14791B7}">
-  <dimension ref="A1:AC79"/>
+  <dimension ref="A1:AC81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1316,33 +1285,31 @@
       <c r="F1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="J1" s="34"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
       <c r="K1" s="23"/>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="26"/>
-      <c r="S1" s="26" t="s">
+      <c r="N1" s="36"/>
+      <c r="S1" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
       <c r="V1" s="6"/>
-      <c r="X1" s="26" t="s">
+      <c r="X1" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" s="26"/>
-      <c r="AB1" s="26" t="s">
+      <c r="Y1" s="36"/>
+      <c r="AB1" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="AC1" s="27"/>
+      <c r="AC1" s="29"/>
     </row>
     <row r="2" spans="1:29" ht="18">
       <c r="A2" s="13"/>
@@ -1355,12 +1322,6 @@
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
-      <c r="I2" t="s">
-        <v>108</v>
-      </c>
-      <c r="J2" t="s">
-        <v>109</v>
-      </c>
       <c r="K2" s="22"/>
       <c r="M2" s="9" t="s">
         <v>65</v>
@@ -1411,15 +1372,10 @@
         <v>28</v>
       </c>
       <c r="G3" s="30"/>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="I3" t="s">
-        <v>107</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>110</v>
-      </c>
+      <c r="J3" s="1"/>
       <c r="K3" s="22"/>
       <c r="M3" s="7" t="s">
         <v>67</v>
@@ -1444,10 +1400,10 @@
         <v>50</v>
       </c>
       <c r="AB3" s="7">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AC3" s="7">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="15.6">
@@ -1470,7 +1426,7 @@
         <v>28</v>
       </c>
       <c r="G4" s="30"/>
-      <c r="H4" s="31"/>
+      <c r="H4" s="27"/>
       <c r="J4" s="1"/>
       <c r="K4" s="22"/>
       <c r="M4" s="7" t="s">
@@ -1520,7 +1476,7 @@
       <c r="G5" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="31"/>
+      <c r="H5" s="27"/>
       <c r="M5" s="7" t="s">
         <v>68</v>
       </c>
@@ -1564,7 +1520,7 @@
         <v>30</v>
       </c>
       <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
+      <c r="H6" s="27"/>
       <c r="M6" s="7" t="s">
         <v>97</v>
       </c>
@@ -1601,7 +1557,7 @@
         <v>30</v>
       </c>
       <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
+      <c r="H7" s="27"/>
       <c r="M7" s="7" t="s">
         <v>98</v>
       </c>
@@ -1637,10 +1593,10 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
       <c r="M8" s="7" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="X8" s="11">
         <v>46012</v>
@@ -1671,10 +1627,10 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
       <c r="M9" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="N9" s="7" t="s">
         <v>155</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>160</v>
       </c>
       <c r="X9" s="11">
         <v>46016</v>
@@ -1695,10 +1651,10 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
       <c r="M10" s="7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="V10" t="s">
         <v>55</v>
@@ -1730,14 +1686,14 @@
         <v>30</v>
       </c>
       <c r="G11" s="30"/>
-      <c r="H11" s="28" t="s">
+      <c r="H11" s="34" t="s">
         <v>39</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="X11" s="11">
         <v>46019</v>
@@ -1766,9 +1722,9 @@
         <v>30</v>
       </c>
       <c r="G12" s="30"/>
-      <c r="H12" s="29"/>
+      <c r="H12" s="35"/>
       <c r="M12" s="7" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="X12" s="11">
         <v>46025</v>
@@ -1781,8 +1737,8 @@
       <c r="A13" s="3">
         <v>46001</v>
       </c>
-      <c r="B13" s="7">
-        <v>8</v>
+      <c r="B13" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>25</v>
@@ -1797,9 +1753,9 @@
       <c r="G13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="29"/>
+      <c r="H13" s="35"/>
       <c r="M13" s="7" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="X13" s="11">
         <v>46026</v>
@@ -1813,7 +1769,7 @@
         <v>46002</v>
       </c>
       <c r="B14" s="7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>7</v>
@@ -1828,7 +1784,7 @@
         <v>30</v>
       </c>
       <c r="G14" s="30"/>
-      <c r="H14" s="29"/>
+      <c r="H14" s="35"/>
       <c r="X14" s="11">
         <v>46032</v>
       </c>
@@ -1841,7 +1797,7 @@
         <v>46003</v>
       </c>
       <c r="B15" s="7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>62</v>
@@ -1856,7 +1812,7 @@
         <v>30</v>
       </c>
       <c r="G15" s="30"/>
-      <c r="H15" s="29"/>
+      <c r="H15" s="35"/>
       <c r="X15" s="11">
         <v>46033</v>
       </c>
@@ -1943,7 +1899,7 @@
         <v>46006</v>
       </c>
       <c r="B19" s="7">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>9</v>
@@ -1958,7 +1914,7 @@
         <v>30</v>
       </c>
       <c r="G19" s="30"/>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="34" t="s">
         <v>74</v>
       </c>
       <c r="N19" s="21"/>
@@ -1974,7 +1930,7 @@
         <v>46007</v>
       </c>
       <c r="B20" s="7">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>4</v>
@@ -1989,7 +1945,7 @@
         <v>30</v>
       </c>
       <c r="G20" s="30"/>
-      <c r="H20" s="29"/>
+      <c r="H20" s="35"/>
       <c r="N20" s="21"/>
       <c r="X20" s="11">
         <v>46053</v>
@@ -2003,7 +1959,7 @@
         <v>46008</v>
       </c>
       <c r="B21" s="7">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>43</v>
@@ -2020,7 +1976,7 @@
       <c r="G21" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="29"/>
+      <c r="H21" s="35"/>
       <c r="N21" s="1"/>
       <c r="X21" s="11">
         <v>46054</v>
@@ -2034,7 +1990,7 @@
         <v>46009</v>
       </c>
       <c r="B22" s="7">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>47</v>
@@ -2051,14 +2007,14 @@
       <c r="G22" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="29"/>
+      <c r="H22" s="35"/>
     </row>
     <row r="23" spans="1:25" ht="15.6">
       <c r="A23" s="3">
         <v>46010</v>
       </c>
       <c r="B23" s="7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>61</v>
@@ -2073,7 +2029,7 @@
         <v>45</v>
       </c>
       <c r="G23" s="30"/>
-      <c r="H23" s="29"/>
+      <c r="H23" s="35"/>
     </row>
     <row r="24" spans="1:25" ht="15.6">
       <c r="A24" s="3">
@@ -2117,7 +2073,7 @@
     </row>
     <row r="26" spans="1:25" ht="18">
       <c r="A26" s="13"/>
-      <c r="B26" s="12"/>
+      <c r="B26" s="7"/>
       <c r="C26" s="9" t="s">
         <v>79</v>
       </c>
@@ -2132,7 +2088,7 @@
         <v>46013</v>
       </c>
       <c r="B27" s="7">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>75</v>
@@ -2147,7 +2103,7 @@
         <v>45</v>
       </c>
       <c r="G27" s="30"/>
-      <c r="H27" s="32" t="s">
+      <c r="H27" s="31" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2156,7 +2112,7 @@
         <v>46014</v>
       </c>
       <c r="B28" s="7">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>75</v>
@@ -2171,14 +2127,14 @@
         <v>45</v>
       </c>
       <c r="G28" s="30"/>
-      <c r="H28" s="33"/>
+      <c r="H28" s="32"/>
     </row>
     <row r="29" spans="1:25" ht="15.6">
       <c r="A29" s="3">
         <v>46015</v>
       </c>
       <c r="B29" s="7">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>87</v>
@@ -2195,7 +2151,7 @@
       <c r="G29" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="H29" s="33"/>
+      <c r="H29" s="32"/>
     </row>
     <row r="30" spans="1:25" ht="15.6">
       <c r="A30" s="3">
@@ -2215,14 +2171,14 @@
       </c>
       <c r="F30" s="13"/>
       <c r="G30" s="30"/>
-      <c r="H30" s="33"/>
+      <c r="H30" s="32"/>
     </row>
     <row r="31" spans="1:25" ht="15.6">
       <c r="A31" s="3">
         <v>46017</v>
       </c>
       <c r="B31" s="7">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>101</v>
@@ -2237,13 +2193,13 @@
         <v>45</v>
       </c>
       <c r="G31" s="30"/>
-      <c r="H31" s="33"/>
+      <c r="H31" s="32"/>
     </row>
     <row r="32" spans="1:25" ht="15.6">
       <c r="A32" s="3">
         <v>46018</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C32" s="7" t="s">
@@ -2263,7 +2219,7 @@
       <c r="A33" s="3">
         <v>46019</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="7" t="s">
@@ -2281,7 +2237,7 @@
     </row>
     <row r="34" spans="1:8" ht="18">
       <c r="A34" s="13"/>
-      <c r="B34" s="12"/>
+      <c r="B34" s="7"/>
       <c r="C34" s="9" t="s">
         <v>80</v>
       </c>
@@ -2296,7 +2252,7 @@
         <v>46020</v>
       </c>
       <c r="B35" s="7">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>93</v>
@@ -2311,7 +2267,7 @@
         <v>45</v>
       </c>
       <c r="G35" s="30"/>
-      <c r="H35" s="32" t="s">
+      <c r="H35" s="31" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2319,8 +2275,8 @@
       <c r="A36" s="3">
         <v>46021</v>
       </c>
-      <c r="B36" s="12">
-        <v>21</v>
+      <c r="B36" s="7">
+        <v>20</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>93</v>
@@ -2335,14 +2291,14 @@
         <v>45</v>
       </c>
       <c r="G36" s="30"/>
-      <c r="H36" s="33"/>
+      <c r="H36" s="32"/>
     </row>
     <row r="37" spans="1:8" ht="15.6">
       <c r="A37" s="3">
         <v>46022</v>
       </c>
-      <c r="B37" s="7">
-        <v>22</v>
+      <c r="B37" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>25</v>
@@ -2357,14 +2313,14 @@
       <c r="G37" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="H37" s="33"/>
+      <c r="H37" s="32"/>
     </row>
     <row r="38" spans="1:8" ht="15.6">
       <c r="A38" s="3">
         <v>46023</v>
       </c>
-      <c r="B38" s="12">
-        <v>23</v>
+      <c r="B38" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>25</v>
@@ -2377,14 +2333,14 @@
       </c>
       <c r="F38" s="13"/>
       <c r="G38" s="30"/>
-      <c r="H38" s="33"/>
+      <c r="H38" s="32"/>
     </row>
     <row r="39" spans="1:8" ht="15.6">
       <c r="A39" s="3">
         <v>46024</v>
       </c>
-      <c r="B39" s="12" t="s">
-        <v>26</v>
+      <c r="B39" s="7">
+        <v>21</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>85</v>
@@ -2399,13 +2355,13 @@
         <v>45</v>
       </c>
       <c r="G39" s="30"/>
-      <c r="H39" s="33"/>
+      <c r="H39" s="32"/>
     </row>
     <row r="40" spans="1:8" ht="15.6">
       <c r="A40" s="3">
         <v>46025</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -2427,7 +2383,7 @@
       <c r="A41" s="3">
         <v>46026</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -2446,7 +2402,7 @@
       <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:8" ht="18">
-      <c r="B42" s="25"/>
+      <c r="B42" s="7"/>
       <c r="C42" s="9" t="s">
         <v>89</v>
       </c>
@@ -2455,8 +2411,8 @@
       <c r="A43" s="3">
         <v>46027</v>
       </c>
-      <c r="B43" s="12">
-        <v>24</v>
+      <c r="B43" s="7">
+        <v>22</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>83</v>
@@ -2471,16 +2427,16 @@
         <v>45</v>
       </c>
       <c r="G43" s="30"/>
-      <c r="H43" s="35" t="s">
-        <v>123</v>
+      <c r="H43" s="26" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.6">
       <c r="A44" s="3">
         <v>46028</v>
       </c>
-      <c r="B44" s="12">
-        <v>25</v>
+      <c r="B44" s="7">
+        <v>23</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>94</v>
@@ -2489,29 +2445,29 @@
         <v>60</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F44" s="13" t="s">
         <v>45</v>
       </c>
       <c r="G44" s="30"/>
-      <c r="H44" s="31"/>
+      <c r="H44" s="27"/>
     </row>
     <row r="45" spans="1:8" ht="15.6">
       <c r="A45" s="3">
         <v>46029</v>
       </c>
-      <c r="B45" s="12">
-        <v>26</v>
+      <c r="B45" s="7">
+        <v>24</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F45" s="13" t="s">
         <v>45</v>
@@ -2519,57 +2475,57 @@
       <c r="G45" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="H45" s="31"/>
+      <c r="H45" s="27"/>
     </row>
     <row r="46" spans="1:8" ht="15.6">
       <c r="A46" s="3">
         <v>46030</v>
       </c>
-      <c r="B46" s="12">
-        <v>27</v>
+      <c r="B46" s="7">
+        <v>25</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="G46" s="27"/>
-      <c r="H46" s="31"/>
+        <v>116</v>
+      </c>
+      <c r="G46" s="29"/>
+      <c r="H46" s="27"/>
     </row>
     <row r="47" spans="1:8" ht="15.6">
       <c r="A47" s="3">
         <v>46031</v>
       </c>
-      <c r="B47" s="12">
-        <v>28</v>
+      <c r="B47" s="7">
+        <v>26</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F47" t="s">
-        <v>121</v>
-      </c>
-      <c r="G47" s="27"/>
-      <c r="H47" s="31"/>
+        <v>116</v>
+      </c>
+      <c r="G47" s="29"/>
+      <c r="H47" s="27"/>
     </row>
     <row r="48" spans="1:8" ht="15.6">
       <c r="A48" s="3">
         <v>46032</v>
       </c>
-      <c r="B48" s="25" t="s">
+      <c r="B48" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C48" s="2" t="s">
@@ -2586,7 +2542,7 @@
       <c r="A49" s="3">
         <v>46033</v>
       </c>
-      <c r="B49" s="25" t="s">
+      <c r="B49" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C49" s="2" t="s">
@@ -2600,117 +2556,123 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="18">
-      <c r="B50" s="25"/>
+      <c r="B50" s="7"/>
       <c r="C50" s="9" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15.6">
       <c r="A51" s="3">
         <v>46034</v>
       </c>
-      <c r="B51" s="25">
-        <v>29</v>
+      <c r="B51" s="7">
+        <v>27</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>60</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F51" t="s">
-        <v>152</v>
-      </c>
-      <c r="H51" s="35" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="H51" s="26" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15.6">
       <c r="A52" s="3">
         <v>46035</v>
       </c>
-      <c r="B52" s="25">
-        <v>30</v>
+      <c r="B52" s="7">
+        <v>28</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F52" t="s">
-        <v>152</v>
-      </c>
-      <c r="H52" s="31"/>
+        <v>147</v>
+      </c>
+      <c r="H52" s="27"/>
     </row>
     <row r="53" spans="1:8" ht="15.6">
       <c r="A53" s="3">
         <v>46036</v>
       </c>
-      <c r="B53" s="25">
-        <v>31</v>
+      <c r="B53" s="7">
+        <v>29</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F53" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="H53" s="31"/>
+        <v>142</v>
+      </c>
+      <c r="H53" s="27"/>
     </row>
     <row r="54" spans="1:8" ht="15.6">
       <c r="A54" s="3">
         <v>46037</v>
       </c>
-      <c r="B54" s="25"/>
+      <c r="B54" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C54" s="2" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="D54" s="25"/>
       <c r="F54" t="s">
-        <v>152</v>
-      </c>
-      <c r="H54" s="31"/>
+        <v>147</v>
+      </c>
+      <c r="H54" s="27"/>
     </row>
     <row r="55" spans="1:8" ht="15.6">
       <c r="A55" s="3">
         <v>46038</v>
       </c>
-      <c r="B55" s="25"/>
+      <c r="B55" s="7">
+        <v>30</v>
+      </c>
       <c r="C55" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E55" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F55" t="s">
-        <v>152</v>
-      </c>
-      <c r="H55" s="31"/>
+        <v>147</v>
+      </c>
+      <c r="H55" s="27"/>
     </row>
     <row r="56" spans="1:8" ht="15.6">
       <c r="A56" s="3">
         <v>46039</v>
       </c>
-      <c r="B56" s="25"/>
+      <c r="B56" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C56" s="2" t="s">
         <v>6</v>
       </c>
@@ -2720,16 +2682,18 @@
       <c r="A57" s="3">
         <v>46040</v>
       </c>
-      <c r="B57" s="25"/>
+      <c r="B57" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C57" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D57" s="25"/>
     </row>
     <row r="58" spans="1:8" ht="18">
-      <c r="B58" s="25"/>
+      <c r="B58" s="7"/>
       <c r="C58" s="9" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D58" s="25"/>
     </row>
@@ -2737,111 +2701,111 @@
       <c r="A59" s="3">
         <v>46041</v>
       </c>
-      <c r="B59" s="25">
-        <v>32</v>
+      <c r="B59" s="7">
+        <v>31</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D59" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F59" t="s">
+        <v>148</v>
+      </c>
+      <c r="H59" s="26" t="s">
         <v>145</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F59" t="s">
-        <v>153</v>
-      </c>
-      <c r="H59" s="35" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="15.6">
       <c r="A60" s="3">
         <v>46042</v>
       </c>
-      <c r="B60" s="25">
-        <v>33</v>
+      <c r="B60" s="7">
+        <v>32</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D60" s="25" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F60" t="s">
-        <v>153</v>
-      </c>
-      <c r="H60" s="35"/>
+        <v>148</v>
+      </c>
+      <c r="H60" s="26"/>
     </row>
     <row r="61" spans="1:8" ht="15.6">
       <c r="A61" s="3">
         <v>46043</v>
       </c>
-      <c r="B61" s="25">
-        <v>34</v>
+      <c r="B61" s="7">
+        <v>33</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D61" s="25" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F61" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="H61" s="35"/>
+        <v>141</v>
+      </c>
+      <c r="H61" s="26"/>
     </row>
     <row r="62" spans="1:8" ht="15.6">
       <c r="A62" s="3">
         <v>46044</v>
       </c>
-      <c r="B62" s="25">
-        <v>35</v>
+      <c r="B62" s="7">
+        <v>34</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F62" t="s">
-        <v>153</v>
-      </c>
-      <c r="H62" s="35"/>
+        <v>148</v>
+      </c>
+      <c r="H62" s="26"/>
     </row>
     <row r="63" spans="1:8" ht="15.6">
       <c r="A63" s="3">
         <v>46045</v>
       </c>
-      <c r="B63" s="25">
-        <v>36</v>
+      <c r="B63" s="7">
+        <v>35</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D63" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="H63" s="35"/>
+      <c r="H63" s="26"/>
     </row>
     <row r="64" spans="1:8" ht="15.6">
       <c r="A64" s="3">
         <v>46046</v>
       </c>
-      <c r="B64" s="25" t="s">
+      <c r="B64" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C64" s="2" t="s">
@@ -2853,7 +2817,7 @@
       <c r="A65" s="3">
         <v>46047</v>
       </c>
-      <c r="B65" s="25" t="s">
+      <c r="B65" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C65" s="2" t="s">
@@ -2862,9 +2826,9 @@
       <c r="D65" s="25"/>
     </row>
     <row r="66" spans="1:8" ht="18">
-      <c r="B66" s="25"/>
+      <c r="B66" s="7"/>
       <c r="C66" s="9" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D66" s="25"/>
     </row>
@@ -2872,109 +2836,109 @@
       <c r="A67" s="3">
         <v>46048</v>
       </c>
-      <c r="B67" s="25">
-        <v>37</v>
+      <c r="B67" s="7">
+        <v>36</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D67" s="25" t="s">
         <v>48</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F67" t="s">
-        <v>154</v>
-      </c>
-      <c r="H67" s="36" t="s">
-        <v>151</v>
+        <v>149</v>
+      </c>
+      <c r="H67" s="28" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="15.6">
       <c r="A68" s="3">
         <v>46049</v>
       </c>
-      <c r="B68" s="25">
-        <v>38</v>
+      <c r="B68" s="7">
+        <v>37</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D68" s="25" t="s">
         <v>48</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F68" t="s">
-        <v>154</v>
-      </c>
-      <c r="H68" s="36"/>
+        <v>149</v>
+      </c>
+      <c r="H68" s="28"/>
     </row>
     <row r="69" spans="1:8" ht="15.6">
       <c r="A69" s="3">
         <v>46050</v>
       </c>
-      <c r="B69" s="25">
-        <v>39</v>
+      <c r="B69" s="7">
+        <v>38</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D69" s="25" t="s">
         <v>48</v>
       </c>
       <c r="E69" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F69" t="s">
+        <v>149</v>
+      </c>
+      <c r="G69" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="F69" t="s">
-        <v>154</v>
-      </c>
-      <c r="G69" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="H69" s="36"/>
+      <c r="H69" s="28"/>
     </row>
     <row r="70" spans="1:8" ht="15.6">
       <c r="A70" s="3">
         <v>46051</v>
       </c>
-      <c r="B70" s="25">
-        <v>40</v>
+      <c r="B70" s="7">
+        <v>39</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D70" s="25" t="s">
         <v>48</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F70" t="s">
-        <v>154</v>
-      </c>
-      <c r="H70" s="36"/>
+        <v>149</v>
+      </c>
+      <c r="H70" s="28"/>
     </row>
     <row r="71" spans="1:8" ht="15.6">
       <c r="A71" s="3">
         <v>46052</v>
       </c>
-      <c r="B71" s="25">
-        <v>41</v>
+      <c r="B71" s="7">
+        <v>40</v>
       </c>
       <c r="C71" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D71" s="25"/>
-      <c r="H71" s="36"/>
+      <c r="H71" s="28"/>
     </row>
     <row r="72" spans="1:8" ht="15.6">
       <c r="A72" s="3">
         <v>46053</v>
       </c>
-      <c r="B72" s="25" t="s">
+      <c r="B72" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C72" s="2" t="s">
@@ -2982,127 +2946,142 @@
       </c>
       <c r="D72" s="25"/>
     </row>
-    <row r="73" spans="1:8" ht="18">
-      <c r="A73" s="3"/>
-      <c r="B73" s="25"/>
-      <c r="C73" s="9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="15.6">
-      <c r="A74" s="3">
+    <row r="73" spans="1:8" ht="15.6">
+      <c r="A73" s="3">
         <v>46054</v>
       </c>
-      <c r="B74" s="25">
-        <v>42</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D74" t="s">
-        <v>164</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F74" t="s">
-        <v>172</v>
+      <c r="B73" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="18">
+      <c r="A74" s="3"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="9" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="15.6">
       <c r="A75" s="3">
-        <v>46055</v>
-      </c>
-      <c r="B75" s="25">
-        <v>43</v>
+        <v>46054</v>
+      </c>
+      <c r="B75" s="7">
+        <v>41</v>
       </c>
       <c r="C75" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D75" t="s">
+        <v>159</v>
+      </c>
+      <c r="E75" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D75" t="s">
-        <v>164</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="F75" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="15.6">
       <c r="A76" s="3">
-        <v>46056</v>
-      </c>
-      <c r="B76" s="25">
-        <v>44</v>
+        <v>46055</v>
+      </c>
+      <c r="B76" s="7">
+        <v>42</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="D76" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F76" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="15.6">
       <c r="A77" s="3">
-        <v>46057</v>
-      </c>
-      <c r="B77" s="25">
-        <v>45</v>
+        <v>46056</v>
+      </c>
+      <c r="B77" s="7">
+        <v>43</v>
       </c>
       <c r="C77" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D77" t="s">
+        <v>161</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F77" t="s">
         <v>167</v>
-      </c>
-      <c r="D77" t="s">
-        <v>166</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F77" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="15.6">
       <c r="A78" s="3">
+        <v>46057</v>
+      </c>
+      <c r="B78" s="7">
+        <v>44</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D78" t="s">
+        <v>161</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F78" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15.6">
+      <c r="A79" s="3">
         <v>46058</v>
       </c>
-      <c r="B78" s="25">
-        <v>46</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D78" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="15.6">
-      <c r="A79" s="3"/>
-      <c r="B79" s="25"/>
+      <c r="B79" s="7">
+        <v>45</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D79" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15.6">
+      <c r="A80" s="3">
+        <v>46059</v>
+      </c>
+      <c r="B80" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15.6">
+      <c r="A81" s="3">
+        <v>46060</v>
+      </c>
+      <c r="B81" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="H51:H55"/>
-    <mergeCell ref="H59:H63"/>
-    <mergeCell ref="H67:H71"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H47"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="H27:H31"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="H11:H15"/>
-    <mergeCell ref="H35:H39"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="H19:H23"/>
     <mergeCell ref="G14:G15"/>
@@ -3116,6 +3095,20 @@
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="H3:H7"/>
     <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H31"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="H11:H15"/>
+    <mergeCell ref="H35:H39"/>
+    <mergeCell ref="H51:H55"/>
+    <mergeCell ref="H59:H63"/>
+    <mergeCell ref="H67:H71"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H47"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" tooltip="Day -7 Blog app create popup and animation" display="https://github.com/AakashChidambaranathan/Intership_task/commit/47e9946674f87f428e5d2cff5875e3cca658dd67" xr:uid="{2740968A-86F6-4ABB-8E7C-25250927D97F}"/>
@@ -3142,826 +3135,32 @@
     <hyperlink ref="E39" r:id="rId22" display="https://github.com/AakashChidambaranathan/Intership_task/tree/c0f18dc48dfe3188a657f8099cc04fcddf58a7e0" xr:uid="{6E53656A-0C82-4E7A-A65A-FDE835A1BA01}"/>
     <hyperlink ref="E35" r:id="rId23" display="https://github.com/AakashChidambaranathan/Intership_task/tree/5e82dcb38869f9dae5bf244ad47810f0bde98f7d" xr:uid="{78FC8660-1532-4FD2-A5B0-37DF01A54746}"/>
     <hyperlink ref="E36" r:id="rId24" display="https://github.com/AakashChidambaranathan/Intership_task/tree/5e82dcb38869f9dae5bf244ad47810f0bde98f7d" xr:uid="{0E926C9D-B86F-4B1F-BF51-A7FC0A9B4678}"/>
-    <hyperlink ref="J3" r:id="rId25" display="https://intership-task-eight.vercel.app/" xr:uid="{ED2C5028-6AA5-4DC1-ACD2-06746E888AB3}"/>
-    <hyperlink ref="E44" r:id="rId26" display="https://github.com/AakashChidambaranathan/Intership_task/tree/18b1e04fd0c68ab22467b44fc88aff51db5fa982" xr:uid="{9F103402-4E1C-4D23-8A4C-A6C23EA37A7D}"/>
-    <hyperlink ref="E45" r:id="rId27" display="https://github.com/AakashChidambaranathan/Intership_task/tree/b84f0708446aca28c8dd19967af2615d517a27a7" xr:uid="{7C7CD810-0E0D-4D05-9C8B-2B100451D532}"/>
-    <hyperlink ref="E46" r:id="rId28" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{411883BD-24F7-40E0-8D73-1D04F1D259BA}"/>
-    <hyperlink ref="E47" r:id="rId29" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{A86CDAB7-7F83-4752-A8E1-29F487667D6B}"/>
-    <hyperlink ref="E51" r:id="rId30" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{AFDC6292-1AD5-4AD7-B44C-FDB7F526A077}"/>
-    <hyperlink ref="E52" r:id="rId31" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{6E66CCA9-20F1-4E4E-B6CC-C64EA357B391}"/>
-    <hyperlink ref="E53" r:id="rId32" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{9C4157E2-7199-47E6-89BC-D137937CA476}"/>
-    <hyperlink ref="E59" r:id="rId33" xr:uid="{2F0C50A4-F41A-4C05-909F-7FAEBF5907EB}"/>
-    <hyperlink ref="E60" r:id="rId34" display="https://github.com/AakashChidambaranathan/Intership_task/tree/2daae779fabe3e1b4a8dbb15b425cf8f38f1447c" xr:uid="{E6AA5D7B-D192-4D1C-AB32-6DCB7F8613CD}"/>
-    <hyperlink ref="E62" r:id="rId35" display="https://github.com/AakashChidambaranathan/Intership_task/tree/ddd3cf7c4973ffcf29e927990c8af509fafabe36" xr:uid="{C0BC58AB-6777-40D9-9317-7797F77D5985}"/>
-    <hyperlink ref="E61" r:id="rId36" xr:uid="{BA236C18-4962-48DA-93A2-8EEFCCC6D72F}"/>
-    <hyperlink ref="E67" r:id="rId37" display="https://github.com/AakashChidambaranathan/Intership_task/tree/bc78e8326ed056418905a04bec214772d22fd6d6" xr:uid="{69A4B7D8-3D1A-4229-B3A5-553690D8FFA3}"/>
-    <hyperlink ref="E69" r:id="rId38" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d75d5b652c9aa4feb2a5a6e08eceae56ed1d474b" xr:uid="{0A1DC9EF-AD5F-4A93-8F17-2E587BD6A4BE}"/>
-    <hyperlink ref="E68" r:id="rId39" display="https://github.com/AakashChidambaranathan/Intership_task/tree/bc78e8326ed056418905a04bec214772d22fd6d6" xr:uid="{3A2701A4-570C-4315-AB4F-C9F1AEF39FC1}"/>
-    <hyperlink ref="E70" r:id="rId40" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d75d5b652c9aa4feb2a5a6e08eceae56ed1d474b" xr:uid="{386EB2F8-A905-48E2-AC95-BADE231F49BC}"/>
-    <hyperlink ref="E74" r:id="rId41" display="https://github.com/AakashChidambaranathan/Intership_task/tree/fe8762988335c451250b807ec80e581a31afdf4a" xr:uid="{B1D32FFB-0B35-48FB-B9AE-9B465BA0D857}"/>
-    <hyperlink ref="E75" r:id="rId42" display="https://github.com/AakashChidambaranathan/Intership_task/tree/47f9d4bc5d85a0eefebb0b6fe213d924a75b9ce1" xr:uid="{963208A8-461D-4FB5-8C16-6BC14618DBE4}"/>
-    <hyperlink ref="E76" r:id="rId43" display="https://github.com/AakashChidambaranathan/Intership_task/tree/687213795ae5372f610365ba9792d521a7c959f9" xr:uid="{553A56B2-C6BA-4287-B777-55FDC5690E1E}"/>
-    <hyperlink ref="E77" r:id="rId44" display="https://github.com/AakashChidambaranathan/Intership_task/tree/01716df1be67fb35d459c6b649e8857cd1b29885" xr:uid="{5EB12A9D-8738-4BBE-97C7-4F523D695CA8}"/>
+    <hyperlink ref="E44" r:id="rId25" display="https://github.com/AakashChidambaranathan/Intership_task/tree/18b1e04fd0c68ab22467b44fc88aff51db5fa982" xr:uid="{9F103402-4E1C-4D23-8A4C-A6C23EA37A7D}"/>
+    <hyperlink ref="E45" r:id="rId26" display="https://github.com/AakashChidambaranathan/Intership_task/tree/b84f0708446aca28c8dd19967af2615d517a27a7" xr:uid="{7C7CD810-0E0D-4D05-9C8B-2B100451D532}"/>
+    <hyperlink ref="E46" r:id="rId27" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{411883BD-24F7-40E0-8D73-1D04F1D259BA}"/>
+    <hyperlink ref="E47" r:id="rId28" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{A86CDAB7-7F83-4752-A8E1-29F487667D6B}"/>
+    <hyperlink ref="E51" r:id="rId29" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{AFDC6292-1AD5-4AD7-B44C-FDB7F526A077}"/>
+    <hyperlink ref="E52" r:id="rId30" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{6E66CCA9-20F1-4E4E-B6CC-C64EA357B391}"/>
+    <hyperlink ref="E53" r:id="rId31" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{9C4157E2-7199-47E6-89BC-D137937CA476}"/>
+    <hyperlink ref="E59" r:id="rId32" xr:uid="{2F0C50A4-F41A-4C05-909F-7FAEBF5907EB}"/>
+    <hyperlink ref="E60" r:id="rId33" display="https://github.com/AakashChidambaranathan/Intership_task/tree/2daae779fabe3e1b4a8dbb15b425cf8f38f1447c" xr:uid="{E6AA5D7B-D192-4D1C-AB32-6DCB7F8613CD}"/>
+    <hyperlink ref="E62" r:id="rId34" display="https://github.com/AakashChidambaranathan/Intership_task/tree/ddd3cf7c4973ffcf29e927990c8af509fafabe36" xr:uid="{C0BC58AB-6777-40D9-9317-7797F77D5985}"/>
+    <hyperlink ref="E61" r:id="rId35" xr:uid="{BA236C18-4962-48DA-93A2-8EEFCCC6D72F}"/>
+    <hyperlink ref="E67" r:id="rId36" display="https://github.com/AakashChidambaranathan/Intership_task/tree/bc78e8326ed056418905a04bec214772d22fd6d6" xr:uid="{69A4B7D8-3D1A-4229-B3A5-553690D8FFA3}"/>
+    <hyperlink ref="E69" r:id="rId37" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d75d5b652c9aa4feb2a5a6e08eceae56ed1d474b" xr:uid="{0A1DC9EF-AD5F-4A93-8F17-2E587BD6A4BE}"/>
+    <hyperlink ref="E68" r:id="rId38" display="https://github.com/AakashChidambaranathan/Intership_task/tree/bc78e8326ed056418905a04bec214772d22fd6d6" xr:uid="{3A2701A4-570C-4315-AB4F-C9F1AEF39FC1}"/>
+    <hyperlink ref="E70" r:id="rId39" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d75d5b652c9aa4feb2a5a6e08eceae56ed1d474b" xr:uid="{386EB2F8-A905-48E2-AC95-BADE231F49BC}"/>
+    <hyperlink ref="E75" r:id="rId40" display="https://github.com/AakashChidambaranathan/Intership_task/tree/fe8762988335c451250b807ec80e581a31afdf4a" xr:uid="{B1D32FFB-0B35-48FB-B9AE-9B465BA0D857}"/>
+    <hyperlink ref="E76" r:id="rId41" display="https://github.com/AakashChidambaranathan/Intership_task/tree/47f9d4bc5d85a0eefebb0b6fe213d924a75b9ce1" xr:uid="{963208A8-461D-4FB5-8C16-6BC14618DBE4}"/>
+    <hyperlink ref="E77" r:id="rId42" display="https://github.com/AakashChidambaranathan/Intership_task/tree/687213795ae5372f610365ba9792d521a7c959f9" xr:uid="{553A56B2-C6BA-4287-B777-55FDC5690E1E}"/>
+    <hyperlink ref="E78" r:id="rId43" display="https://github.com/AakashChidambaranathan/Intership_task/tree/01716df1be67fb35d459c6b649e8857cd1b29885" xr:uid="{5EB12A9D-8738-4BBE-97C7-4F523D695CA8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId45"/>
+  <pageSetup orientation="portrait" r:id="rId44"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8849BD1A-5B5D-47AB-A398-D3AB96A31B76}">
-  <dimension ref="A1:AC39"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" customWidth="1"/>
-    <col min="3" max="3" width="56.109375" customWidth="1"/>
-    <col min="4" max="4" width="57.6640625" customWidth="1"/>
-    <col min="5" max="5" width="37.6640625" customWidth="1"/>
-    <col min="6" max="6" width="45.88671875" customWidth="1"/>
-    <col min="7" max="7" width="33.33203125" customWidth="1"/>
-    <col min="8" max="8" width="36.44140625" customWidth="1"/>
-    <col min="27" max="27" width="13.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" ht="18">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="23"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="6"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="27"/>
-    </row>
-    <row r="2" spans="1:29" ht="15.6">
-      <c r="A2" s="3">
-        <v>46020</v>
-      </c>
-      <c r="B2" s="7">
-        <v>20</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="32" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" ht="15.6">
-      <c r="A3" s="3">
-        <v>46021</v>
-      </c>
-      <c r="B3" s="12">
-        <v>21</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="33"/>
-    </row>
-    <row r="4" spans="1:29" ht="15.6">
-      <c r="A4" s="3">
-        <v>46022</v>
-      </c>
-      <c r="B4" s="7">
-        <v>22</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H4" s="33"/>
-    </row>
-    <row r="5" spans="1:29" ht="15.6">
-      <c r="A5" s="3">
-        <v>46023</v>
-      </c>
-      <c r="B5" s="12">
-        <v>23</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="33"/>
-    </row>
-    <row r="6" spans="1:29" ht="15.6">
-      <c r="A6" s="3">
-        <v>46024</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="33"/>
-    </row>
-    <row r="7" spans="1:29" ht="15.6">
-      <c r="A7" s="3">
-        <v>46025</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-    </row>
-    <row r="8" spans="1:29" ht="15.6">
-      <c r="A8" s="3">
-        <v>46026</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-    </row>
-    <row r="9" spans="1:29" ht="18">
-      <c r="B9" s="25"/>
-      <c r="C9" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" ht="15.6">
-      <c r="A10" s="3">
-        <v>46027</v>
-      </c>
-      <c r="B10" s="12">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="30"/>
-      <c r="H10" s="35" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" ht="15.6">
-      <c r="A11" s="3">
-        <v>46028</v>
-      </c>
-      <c r="B11" s="12">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="31"/>
-    </row>
-    <row r="12" spans="1:29" ht="15.6">
-      <c r="A12" s="3">
-        <v>46029</v>
-      </c>
-      <c r="B12" s="12">
-        <v>26</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="H12" s="31"/>
-    </row>
-    <row r="13" spans="1:29" ht="15.6">
-      <c r="A13" s="3">
-        <v>46030</v>
-      </c>
-      <c r="B13" s="12">
-        <v>27</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="G13" s="27"/>
-      <c r="H13" s="31"/>
-    </row>
-    <row r="14" spans="1:29" ht="15.6">
-      <c r="A14" s="3">
-        <v>46031</v>
-      </c>
-      <c r="B14" s="12">
-        <v>28</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F14" t="s">
-        <v>121</v>
-      </c>
-      <c r="G14" s="27"/>
-      <c r="H14" s="31"/>
-    </row>
-    <row r="15" spans="1:29" ht="15.6">
-      <c r="A15" s="3">
-        <v>46032</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" ht="15.6">
-      <c r="A16" s="3">
-        <v>46033</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="18">
-      <c r="B17" s="25"/>
-      <c r="C17" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.6">
-      <c r="A18" s="3">
-        <v>46034</v>
-      </c>
-      <c r="B18" s="25">
-        <v>29</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F18" t="s">
-        <v>152</v>
-      </c>
-      <c r="H18" s="35" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.6">
-      <c r="A19" s="3">
-        <v>46035</v>
-      </c>
-      <c r="B19" s="25">
-        <v>30</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F19" t="s">
-        <v>152</v>
-      </c>
-      <c r="H19" s="31"/>
-    </row>
-    <row r="20" spans="1:8" ht="15.6">
-      <c r="A20" s="3">
-        <v>46036</v>
-      </c>
-      <c r="B20" s="25">
-        <v>31</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F20" t="s">
-        <v>152</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="H20" s="31"/>
-    </row>
-    <row r="21" spans="1:8" ht="15.6">
-      <c r="A21" s="3">
-        <v>46037</v>
-      </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="25"/>
-      <c r="F21" t="s">
-        <v>152</v>
-      </c>
-      <c r="H21" s="31"/>
-    </row>
-    <row r="22" spans="1:8" ht="15.6">
-      <c r="A22" s="3">
-        <v>46038</v>
-      </c>
-      <c r="B22" s="25">
-        <v>32</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E22" t="s">
-        <v>119</v>
-      </c>
-      <c r="F22" t="s">
-        <v>152</v>
-      </c>
-      <c r="H22" s="31"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.6">
-      <c r="A23" s="3">
-        <v>46039</v>
-      </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="25"/>
-    </row>
-    <row r="24" spans="1:8" ht="15.6">
-      <c r="A24" s="3">
-        <v>46040</v>
-      </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="25"/>
-    </row>
-    <row r="25" spans="1:8" ht="18">
-      <c r="B25" s="25"/>
-      <c r="C25" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D25" s="25"/>
-    </row>
-    <row r="26" spans="1:8" ht="15.6">
-      <c r="A26" s="3">
-        <v>46041</v>
-      </c>
-      <c r="B26" s="25">
-        <v>33</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F26" t="s">
-        <v>153</v>
-      </c>
-      <c r="H26" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.6">
-      <c r="A27" s="3">
-        <v>46042</v>
-      </c>
-      <c r="B27" s="25">
-        <v>34</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F27" t="s">
-        <v>153</v>
-      </c>
-      <c r="H27" s="35"/>
-    </row>
-    <row r="28" spans="1:8" ht="15.6">
-      <c r="A28" s="3">
-        <v>46043</v>
-      </c>
-      <c r="B28" s="25">
-        <v>35</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F28" t="s">
-        <v>153</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="H28" s="35"/>
-    </row>
-    <row r="29" spans="1:8" ht="15.6">
-      <c r="A29" s="3">
-        <v>46044</v>
-      </c>
-      <c r="B29" s="25">
-        <v>36</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F29" t="s">
-        <v>153</v>
-      </c>
-      <c r="H29" s="35"/>
-    </row>
-    <row r="30" spans="1:8" ht="15.6">
-      <c r="A30" s="3">
-        <v>46045</v>
-      </c>
-      <c r="B30" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="D30" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="H30" s="35"/>
-    </row>
-    <row r="31" spans="1:8" ht="15.6">
-      <c r="A31" s="3">
-        <v>46046</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="25"/>
-    </row>
-    <row r="32" spans="1:8" ht="15.6">
-      <c r="A32" s="3">
-        <v>46047</v>
-      </c>
-      <c r="B32" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="25"/>
-    </row>
-    <row r="33" spans="1:8" ht="18">
-      <c r="B33" s="25"/>
-      <c r="C33" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D33" s="25"/>
-    </row>
-    <row r="34" spans="1:8" ht="15.6">
-      <c r="A34" s="3">
-        <v>46048</v>
-      </c>
-      <c r="B34" s="25">
-        <v>37</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F34" t="s">
-        <v>154</v>
-      </c>
-      <c r="H34" s="36" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="15.6">
-      <c r="A35" s="3">
-        <v>46049</v>
-      </c>
-      <c r="B35" s="25">
-        <v>38</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="D35" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F35" t="s">
-        <v>154</v>
-      </c>
-      <c r="H35" s="36"/>
-    </row>
-    <row r="36" spans="1:8" ht="15.6">
-      <c r="A36" s="3">
-        <v>46050</v>
-      </c>
-      <c r="B36" s="25">
-        <v>39</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D36" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F36" t="s">
-        <v>154</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="H36" s="36"/>
-    </row>
-    <row r="37" spans="1:8" ht="15.6">
-      <c r="A37" s="3">
-        <v>46051</v>
-      </c>
-      <c r="B37" s="25">
-        <v>34</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D37" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F37" t="s">
-        <v>154</v>
-      </c>
-      <c r="H37" s="36"/>
-    </row>
-    <row r="38" spans="1:8" ht="15.6">
-      <c r="A38" s="3">
-        <v>46052</v>
-      </c>
-      <c r="B38" s="25">
-        <v>35</v>
-      </c>
-      <c r="C38" t="s">
-        <v>144</v>
-      </c>
-      <c r="D38" s="25"/>
-      <c r="H38" s="36"/>
-    </row>
-    <row r="39" spans="1:8" ht="15.6">
-      <c r="A39" s="3">
-        <v>46053</v>
-      </c>
-      <c r="B39" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H18:H22"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="H26:H30"/>
-    <mergeCell ref="H34:H38"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="M1:N1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="E10" r:id="rId1" display="https://github.com/AakashChidambaranathan/Intership_task/tree/9135683980ad23825bb62e52e371e0f6e3c013c4" xr:uid="{8318D3D4-2ED6-43C8-BABA-00D454BA9CEC}"/>
-    <hyperlink ref="E6" r:id="rId2" display="https://github.com/AakashChidambaranathan/Intership_task/tree/c0f18dc48dfe3188a657f8099cc04fcddf58a7e0" xr:uid="{CD27853E-FF92-4529-8414-4AC4B1FE09F1}"/>
-    <hyperlink ref="E2" r:id="rId3" display="https://github.com/AakashChidambaranathan/Intership_task/tree/5e82dcb38869f9dae5bf244ad47810f0bde98f7d" xr:uid="{41A44120-6327-4AA9-AA08-1E26904FFB8F}"/>
-    <hyperlink ref="E3" r:id="rId4" display="https://github.com/AakashChidambaranathan/Intership_task/tree/5e82dcb38869f9dae5bf244ad47810f0bde98f7d" xr:uid="{FA38B619-5A4F-4199-ACF1-487F894EA461}"/>
-    <hyperlink ref="E11" r:id="rId5" display="https://github.com/AakashChidambaranathan/Intership_task/tree/18b1e04fd0c68ab22467b44fc88aff51db5fa982" xr:uid="{674501F0-5607-42B0-A077-21C37AEDC1D3}"/>
-    <hyperlink ref="E12" r:id="rId6" display="https://github.com/AakashChidambaranathan/Intership_task/tree/b84f0708446aca28c8dd19967af2615d517a27a7" xr:uid="{CC98102C-0588-4405-8FC2-C208039E9829}"/>
-    <hyperlink ref="E13" r:id="rId7" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{ACCFB52B-8469-4A01-BB12-1072CB2E7D4A}"/>
-    <hyperlink ref="E14" r:id="rId8" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{3401966F-BBC0-4556-A8B2-8BC39D97B489}"/>
-    <hyperlink ref="E18" r:id="rId9" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{7FFE6E63-6412-42E8-9F96-614703015438}"/>
-    <hyperlink ref="E19" r:id="rId10" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{83AB7E3D-3A5E-4FFE-BB5E-9D91C52146E7}"/>
-    <hyperlink ref="E20" r:id="rId11" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{224EF37E-E606-4C2F-AFBD-251FA38DFEA9}"/>
-    <hyperlink ref="E26" r:id="rId12" xr:uid="{77E67683-D0D9-4AA0-B028-6BC935385AF1}"/>
-    <hyperlink ref="E27" r:id="rId13" display="https://github.com/AakashChidambaranathan/Intership_task/tree/2daae779fabe3e1b4a8dbb15b425cf8f38f1447c" xr:uid="{EA1C0276-1B38-4884-B5B2-041BF1C15F2F}"/>
-    <hyperlink ref="E29" r:id="rId14" display="https://github.com/AakashChidambaranathan/Intership_task/tree/ddd3cf7c4973ffcf29e927990c8af509fafabe36" xr:uid="{C245925B-1D76-48C2-ACAD-F70FFF162A80}"/>
-    <hyperlink ref="E28" r:id="rId15" xr:uid="{9AE3D071-6833-4623-94E2-DAEDC1AB9975}"/>
-    <hyperlink ref="E34" r:id="rId16" display="https://github.com/AakashChidambaranathan/Intership_task/tree/bc78e8326ed056418905a04bec214772d22fd6d6" xr:uid="{570ECD13-D24A-4642-B30F-32E14DE13364}"/>
-    <hyperlink ref="E36" r:id="rId17" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d75d5b652c9aa4feb2a5a6e08eceae56ed1d474b" xr:uid="{DC60E8A4-6486-4A12-ACBB-9C7FD4FB4C9B}"/>
-    <hyperlink ref="E35" r:id="rId18" display="https://github.com/AakashChidambaranathan/Intership_task/tree/bc78e8326ed056418905a04bec214772d22fd6d6" xr:uid="{913FA76D-52EB-4FDD-B2B5-2271A634C455}"/>
-    <hyperlink ref="E37" r:id="rId19" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d75d5b652c9aa4feb2a5a6e08eceae56ed1d474b" xr:uid="{E3534CB4-D159-4F79-9E70-E8559F578C8B}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E3E4F9-9B7C-4166-B756-1C0E93C0BC1D}">
   <dimension ref="A1:K46"/>
   <sheetViews>
@@ -4000,10 +3199,10 @@
       <c r="F1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="26"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="2" spans="1:8" ht="18">
       <c r="A2" s="13"/>
@@ -4037,7 +3236,7 @@
         <v>28</v>
       </c>
       <c r="G3" s="30"/>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="34" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4061,7 +3260,7 @@
         <v>28</v>
       </c>
       <c r="G4" s="30"/>
-      <c r="H4" s="31"/>
+      <c r="H4" s="27"/>
     </row>
     <row r="5" spans="1:8" ht="15.6">
       <c r="A5" s="3">
@@ -4085,7 +3284,7 @@
       <c r="G5" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="31"/>
+      <c r="H5" s="27"/>
     </row>
     <row r="6" spans="1:8" ht="15.6">
       <c r="A6" s="3">
@@ -4107,7 +3306,7 @@
         <v>30</v>
       </c>
       <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
+      <c r="H6" s="27"/>
     </row>
     <row r="7" spans="1:8" ht="15.6">
       <c r="A7" s="3">
@@ -4129,7 +3328,7 @@
         <v>30</v>
       </c>
       <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
+      <c r="H7" s="27"/>
     </row>
     <row r="8" spans="1:8" ht="15.6">
       <c r="A8" s="3">
@@ -4207,7 +3406,7 @@
         <v>30</v>
       </c>
       <c r="G11" s="30"/>
-      <c r="H11" s="28" t="s">
+      <c r="H11" s="34" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4231,7 +3430,7 @@
         <v>30</v>
       </c>
       <c r="G12" s="30"/>
-      <c r="H12" s="29"/>
+      <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:8" ht="15.6">
       <c r="A13" s="3">
@@ -4253,7 +3452,7 @@
       <c r="G13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="29"/>
+      <c r="H13" s="35"/>
     </row>
     <row r="14" spans="1:8" ht="15.6">
       <c r="A14" s="3">
@@ -4275,7 +3474,7 @@
         <v>30</v>
       </c>
       <c r="G14" s="30"/>
-      <c r="H14" s="29"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="1:8" ht="15.6">
       <c r="A15" s="3">
@@ -4297,7 +3496,7 @@
         <v>30</v>
       </c>
       <c r="G15" s="30"/>
-      <c r="H15" s="29"/>
+      <c r="H15" s="35"/>
     </row>
     <row r="16" spans="1:8" ht="15.6">
       <c r="A16" s="3">
@@ -4885,6 +4084,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H15"/>
+    <mergeCell ref="G14:G15"/>
     <mergeCell ref="G35:G36"/>
     <mergeCell ref="H35:H39"/>
     <mergeCell ref="G38:G39"/>
@@ -4894,13 +4100,6 @@
     <mergeCell ref="G27:G28"/>
     <mergeCell ref="H27:H31"/>
     <mergeCell ref="G30:G31"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H15"/>
-    <mergeCell ref="G14:G15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" tooltip="Day -7 Blog app create popup and animation" display="https://github.com/AakashChidambaranathan/Intership_task/commit/47e9946674f87f428e5d2cff5875e3cca658dd67" xr:uid="{E6BF1654-2E60-4C7B-8C06-71168BF228BE}"/>
@@ -4930,6 +4129,799 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8849BD1A-5B5D-47AB-A398-D3AB96A31B76}">
+  <dimension ref="A1:AC39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="70" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" customWidth="1"/>
+    <col min="3" max="3" width="56.109375" customWidth="1"/>
+    <col min="4" max="4" width="57.6640625" customWidth="1"/>
+    <col min="5" max="5" width="37.6640625" customWidth="1"/>
+    <col min="6" max="6" width="45.88671875" customWidth="1"/>
+    <col min="7" max="7" width="33.33203125" customWidth="1"/>
+    <col min="8" max="8" width="36.44140625" customWidth="1"/>
+    <col min="27" max="27" width="13.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" ht="18">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="36"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="23"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="6"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="29"/>
+    </row>
+    <row r="2" spans="1:29" ht="15.6">
+      <c r="A2" s="3">
+        <v>46020</v>
+      </c>
+      <c r="B2" s="7">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="15.6">
+      <c r="A3" s="3">
+        <v>46021</v>
+      </c>
+      <c r="B3" s="12">
+        <v>21</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="30"/>
+      <c r="H3" s="32"/>
+    </row>
+    <row r="4" spans="1:29" ht="15.6">
+      <c r="A4" s="3">
+        <v>46022</v>
+      </c>
+      <c r="B4" s="7">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="32"/>
+    </row>
+    <row r="5" spans="1:29" ht="15.6">
+      <c r="A5" s="3">
+        <v>46023</v>
+      </c>
+      <c r="B5" s="12">
+        <v>23</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="32"/>
+    </row>
+    <row r="6" spans="1:29" ht="15.6">
+      <c r="A6" s="3">
+        <v>46024</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="30"/>
+      <c r="H6" s="32"/>
+    </row>
+    <row r="7" spans="1:29" ht="15.6">
+      <c r="A7" s="3">
+        <v>46025</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:29" ht="15.6">
+      <c r="A8" s="3">
+        <v>46026</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:29" ht="18">
+      <c r="B9" s="25"/>
+      <c r="C9" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="15.6">
+      <c r="A10" s="3">
+        <v>46027</v>
+      </c>
+      <c r="B10" s="12">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="30"/>
+      <c r="H10" s="26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="15.6">
+      <c r="A11" s="3">
+        <v>46028</v>
+      </c>
+      <c r="B11" s="12">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="30"/>
+      <c r="H11" s="27"/>
+    </row>
+    <row r="12" spans="1:29" ht="15.6">
+      <c r="A12" s="3">
+        <v>46029</v>
+      </c>
+      <c r="B12" s="12">
+        <v>26</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="27"/>
+    </row>
+    <row r="13" spans="1:29" ht="15.6">
+      <c r="A13" s="3">
+        <v>46030</v>
+      </c>
+      <c r="B13" s="12">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" s="29"/>
+      <c r="H13" s="27"/>
+    </row>
+    <row r="14" spans="1:29" ht="15.6">
+      <c r="A14" s="3">
+        <v>46031</v>
+      </c>
+      <c r="B14" s="12">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G14" s="29"/>
+      <c r="H14" s="27"/>
+    </row>
+    <row r="15" spans="1:29" ht="15.6">
+      <c r="A15" s="3">
+        <v>46032</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" ht="15.6">
+      <c r="A16" s="3">
+        <v>46033</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="18">
+      <c r="B17" s="25"/>
+      <c r="C17" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.6">
+      <c r="A18" s="3">
+        <v>46034</v>
+      </c>
+      <c r="B18" s="25">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" t="s">
+        <v>147</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.6">
+      <c r="A19" s="3">
+        <v>46035</v>
+      </c>
+      <c r="B19" s="25">
+        <v>30</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F19" t="s">
+        <v>147</v>
+      </c>
+      <c r="H19" s="27"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.6">
+      <c r="A20" s="3">
+        <v>46036</v>
+      </c>
+      <c r="B20" s="25">
+        <v>31</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" t="s">
+        <v>147</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H20" s="27"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.6">
+      <c r="A21" s="3">
+        <v>46037</v>
+      </c>
+      <c r="B21" s="25"/>
+      <c r="C21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="25"/>
+      <c r="F21" t="s">
+        <v>147</v>
+      </c>
+      <c r="H21" s="27"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.6">
+      <c r="A22" s="3">
+        <v>46038</v>
+      </c>
+      <c r="B22" s="25">
+        <v>32</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" t="s">
+        <v>147</v>
+      </c>
+      <c r="H22" s="27"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.6">
+      <c r="A23" s="3">
+        <v>46039</v>
+      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="25"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.6">
+      <c r="A24" s="3">
+        <v>46040</v>
+      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="25"/>
+    </row>
+    <row r="25" spans="1:8" ht="18">
+      <c r="B25" s="25"/>
+      <c r="C25" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" s="25"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.6">
+      <c r="A26" s="3">
+        <v>46041</v>
+      </c>
+      <c r="B26" s="25">
+        <v>33</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F26" t="s">
+        <v>148</v>
+      </c>
+      <c r="H26" s="26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.6">
+      <c r="A27" s="3">
+        <v>46042</v>
+      </c>
+      <c r="B27" s="25">
+        <v>34</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F27" t="s">
+        <v>148</v>
+      </c>
+      <c r="H27" s="26"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.6">
+      <c r="A28" s="3">
+        <v>46043</v>
+      </c>
+      <c r="B28" s="25">
+        <v>35</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" t="s">
+        <v>148</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H28" s="26"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.6">
+      <c r="A29" s="3">
+        <v>46044</v>
+      </c>
+      <c r="B29" s="25">
+        <v>36</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F29" t="s">
+        <v>148</v>
+      </c>
+      <c r="H29" s="26"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.6">
+      <c r="A30" s="3">
+        <v>46045</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" s="26"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.6">
+      <c r="A31" s="3">
+        <v>46046</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="25"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.6">
+      <c r="A32" s="3">
+        <v>46047</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="25"/>
+    </row>
+    <row r="33" spans="1:8" ht="18">
+      <c r="B33" s="25"/>
+      <c r="C33" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D33" s="25"/>
+    </row>
+    <row r="34" spans="1:8" ht="15.6">
+      <c r="A34" s="3">
+        <v>46048</v>
+      </c>
+      <c r="B34" s="25">
+        <v>37</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F34" t="s">
+        <v>149</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.6">
+      <c r="A35" s="3">
+        <v>46049</v>
+      </c>
+      <c r="B35" s="25">
+        <v>38</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F35" t="s">
+        <v>149</v>
+      </c>
+      <c r="H35" s="28"/>
+    </row>
+    <row r="36" spans="1:8" ht="15.6">
+      <c r="A36" s="3">
+        <v>46050</v>
+      </c>
+      <c r="B36" s="25">
+        <v>39</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F36" t="s">
+        <v>149</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="H36" s="28"/>
+    </row>
+    <row r="37" spans="1:8" ht="15.6">
+      <c r="A37" s="3">
+        <v>46051</v>
+      </c>
+      <c r="B37" s="25">
+        <v>34</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F37" t="s">
+        <v>149</v>
+      </c>
+      <c r="H37" s="28"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.6">
+      <c r="A38" s="3">
+        <v>46052</v>
+      </c>
+      <c r="B38" s="25">
+        <v>35</v>
+      </c>
+      <c r="C38" t="s">
+        <v>139</v>
+      </c>
+      <c r="D38" s="25"/>
+      <c r="H38" s="28"/>
+    </row>
+    <row r="39" spans="1:8" ht="15.6">
+      <c r="A39" s="3">
+        <v>46053</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="H26:H30"/>
+    <mergeCell ref="H34:H38"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H18:H22"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H6"/>
+    <mergeCell ref="G5:G6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E10" r:id="rId1" display="https://github.com/AakashChidambaranathan/Intership_task/tree/9135683980ad23825bb62e52e371e0f6e3c013c4" xr:uid="{8318D3D4-2ED6-43C8-BABA-00D454BA9CEC}"/>
+    <hyperlink ref="E6" r:id="rId2" display="https://github.com/AakashChidambaranathan/Intership_task/tree/c0f18dc48dfe3188a657f8099cc04fcddf58a7e0" xr:uid="{CD27853E-FF92-4529-8414-4AC4B1FE09F1}"/>
+    <hyperlink ref="E2" r:id="rId3" display="https://github.com/AakashChidambaranathan/Intership_task/tree/5e82dcb38869f9dae5bf244ad47810f0bde98f7d" xr:uid="{41A44120-6327-4AA9-AA08-1E26904FFB8F}"/>
+    <hyperlink ref="E3" r:id="rId4" display="https://github.com/AakashChidambaranathan/Intership_task/tree/5e82dcb38869f9dae5bf244ad47810f0bde98f7d" xr:uid="{FA38B619-5A4F-4199-ACF1-487F894EA461}"/>
+    <hyperlink ref="E11" r:id="rId5" display="https://github.com/AakashChidambaranathan/Intership_task/tree/18b1e04fd0c68ab22467b44fc88aff51db5fa982" xr:uid="{674501F0-5607-42B0-A077-21C37AEDC1D3}"/>
+    <hyperlink ref="E12" r:id="rId6" display="https://github.com/AakashChidambaranathan/Intership_task/tree/b84f0708446aca28c8dd19967af2615d517a27a7" xr:uid="{CC98102C-0588-4405-8FC2-C208039E9829}"/>
+    <hyperlink ref="E13" r:id="rId7" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{ACCFB52B-8469-4A01-BB12-1072CB2E7D4A}"/>
+    <hyperlink ref="E14" r:id="rId8" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{3401966F-BBC0-4556-A8B2-8BC39D97B489}"/>
+    <hyperlink ref="E18" r:id="rId9" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{7FFE6E63-6412-42E8-9F96-614703015438}"/>
+    <hyperlink ref="E19" r:id="rId10" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{83AB7E3D-3A5E-4FFE-BB5E-9D91C52146E7}"/>
+    <hyperlink ref="E20" r:id="rId11" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d67f0f0b04a023ddfcfb0772c2b7504ebfb1d620" xr:uid="{224EF37E-E606-4C2F-AFBD-251FA38DFEA9}"/>
+    <hyperlink ref="E26" r:id="rId12" xr:uid="{77E67683-D0D9-4AA0-B028-6BC935385AF1}"/>
+    <hyperlink ref="E27" r:id="rId13" display="https://github.com/AakashChidambaranathan/Intership_task/tree/2daae779fabe3e1b4a8dbb15b425cf8f38f1447c" xr:uid="{EA1C0276-1B38-4884-B5B2-041BF1C15F2F}"/>
+    <hyperlink ref="E29" r:id="rId14" display="https://github.com/AakashChidambaranathan/Intership_task/tree/ddd3cf7c4973ffcf29e927990c8af509fafabe36" xr:uid="{C245925B-1D76-48C2-ACAD-F70FFF162A80}"/>
+    <hyperlink ref="E28" r:id="rId15" xr:uid="{9AE3D071-6833-4623-94E2-DAEDC1AB9975}"/>
+    <hyperlink ref="E34" r:id="rId16" display="https://github.com/AakashChidambaranathan/Intership_task/tree/bc78e8326ed056418905a04bec214772d22fd6d6" xr:uid="{570ECD13-D24A-4642-B30F-32E14DE13364}"/>
+    <hyperlink ref="E36" r:id="rId17" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d75d5b652c9aa4feb2a5a6e08eceae56ed1d474b" xr:uid="{DC60E8A4-6486-4A12-ACBB-9C7FD4FB4C9B}"/>
+    <hyperlink ref="E35" r:id="rId18" display="https://github.com/AakashChidambaranathan/Intership_task/tree/bc78e8326ed056418905a04bec214772d22fd6d6" xr:uid="{913FA76D-52EB-4FDD-B2B5-2271A634C455}"/>
+    <hyperlink ref="E37" r:id="rId19" display="https://github.com/AakashChidambaranathan/Intership_task/tree/d75d5b652c9aa4feb2a5a6e08eceae56ed1d474b" xr:uid="{E3534CB4-D159-4F79-9E70-E8559F578C8B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E91C5E-F27B-41D1-8BA2-ADBA109D0125}">
   <dimension ref="A1:C10"/>
@@ -4996,14 +4988,14 @@
         <v>99</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="41"/>
       <c r="B7" s="41"/>
       <c r="C7" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="31.2">
@@ -5049,20 +5041,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17.399999999999999">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
       <c r="D1" s="6"/>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="26"/>
-      <c r="J1" s="26" t="s">
+      <c r="G1" s="36"/>
+      <c r="J1" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="K1" s="27"/>
+      <c r="K1" s="29"/>
     </row>
     <row r="2" spans="1:11" ht="17.399999999999999">
       <c r="A2" s="8" t="s">

</xml_diff>